<commit_message>
updated business case excel file
</commit_message>
<xml_diff>
--- a/mppsteel/data/import_data/Business Cases One Table.xlsx
+++ b/mppsteel/data/import_data/Business Cases One Table.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="24527"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="24701"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://systemiq.sharepoint.com/Projects/MPP0006/Shared Documents/6_ Working documents/03 Steel python model/Data Sources/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="1625" documentId="8_{E5ECF8DE-F7F7-4DAE-A1FD-DC27A0AAFB42}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{A233D31D-566A-4C2B-A564-4DBF5B3656C4}"/>
+  <xr:revisionPtr revIDLastSave="1655" documentId="8_{E5ECF8DE-F7F7-4DAE-A1FD-DC27A0AAFB42}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{D797A1E5-9EE8-4A0C-916F-535336CC4417}"/>
   <bookViews>
-    <workbookView xWindow="-93" yWindow="-93" windowWidth="25786" windowHeight="13373" xr2:uid="{0B6EB920-BFAC-40B8-A9D9-6AEA75F19191}"/>
+    <workbookView xWindow="28680" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{0B6EB920-BFAC-40B8-A9D9-6AEA75F19191}"/>
   </bookViews>
   <sheets>
     <sheet name="Data" sheetId="1" r:id="rId1"/>
@@ -91,7 +91,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="821" uniqueCount="176">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="821" uniqueCount="175">
   <si>
     <t>Steel Business Cases</t>
   </si>
@@ -345,9 +345,6 @@
     <t>Solid fuels</t>
   </si>
   <si>
-    <t xml:space="preserve">Biomethane </t>
-  </si>
-  <si>
     <t>Blast Furnace</t>
   </si>
   <si>
@@ -459,9 +456,6 @@
     <t>Captured CO2</t>
   </si>
   <si>
-    <t>25 MW Steel</t>
-  </si>
-  <si>
     <t>Electrolyzer</t>
   </si>
   <si>
@@ -619,6 +613,9 @@
   </si>
   <si>
     <t>Iron heat of fusion</t>
+  </si>
+  <si>
+    <t>Power consumption for oxygen separation in ASU</t>
   </si>
 </sst>
 </file>
@@ -628,7 +625,7 @@
   <numFmts count="1">
     <numFmt numFmtId="164" formatCode="0.000"/>
   </numFmts>
-  <fonts count="9" x14ac:knownFonts="1">
+  <fonts count="9">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -1122,47 +1119,46 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{F5E4BE5B-48FB-4F9E-83ED-5B539B3F5C30}">
-  <sheetPr filterMode="1"/>
   <dimension ref="A1:AB161"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="80" zoomScaleNormal="80" workbookViewId="0">
-      <pane xSplit="6" ySplit="2" topLeftCell="G3" activePane="bottomRight" state="frozen"/>
+    <sheetView tabSelected="1" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
+      <pane xSplit="6" ySplit="2" topLeftCell="G111" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="G1" sqref="G1"/>
       <selection pane="bottomLeft" activeCell="A4" sqref="A4"/>
-      <selection pane="bottomRight" activeCell="D10" sqref="D10"/>
+      <selection pane="bottomRight" activeCell="D136" sqref="D136"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.35" x14ac:dyDescent="0.5"/>
+  <sheetFormatPr defaultRowHeight="14.5"/>
   <cols>
     <col min="1" max="1" width="25" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="30.52734375" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="30.52734375" customWidth="1"/>
-    <col min="4" max="4" width="39.52734375" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="30.54296875" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="30.54296875" customWidth="1"/>
+    <col min="4" max="4" width="39.54296875" bestFit="1" customWidth="1"/>
     <col min="5" max="5" width="26" customWidth="1"/>
-    <col min="6" max="6" width="17.29296875" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="7.52734375" customWidth="1"/>
-    <col min="8" max="8" width="9.17578125" style="9" customWidth="1"/>
-    <col min="9" max="9" width="14.17578125" style="9" bestFit="1" customWidth="1"/>
-    <col min="10" max="10" width="11.17578125" style="9" bestFit="1" customWidth="1"/>
-    <col min="11" max="11" width="14.17578125" style="9" bestFit="1" customWidth="1"/>
-    <col min="12" max="12" width="11.17578125" style="9" bestFit="1" customWidth="1"/>
-    <col min="13" max="16" width="9.17578125" style="9" customWidth="1"/>
-    <col min="17" max="17" width="9.703125" style="9" bestFit="1" customWidth="1"/>
-    <col min="18" max="19" width="11.17578125" style="9" bestFit="1" customWidth="1"/>
-    <col min="20" max="20" width="9.17578125" style="9" customWidth="1"/>
-    <col min="21" max="21" width="14.17578125" style="9" bestFit="1" customWidth="1"/>
-    <col min="22" max="22" width="11.17578125" style="9" bestFit="1" customWidth="1"/>
-    <col min="23" max="23" width="14.17578125" style="9" bestFit="1" customWidth="1"/>
-    <col min="24" max="26" width="9.17578125" style="9" customWidth="1"/>
-    <col min="27" max="27" width="11.17578125" style="9" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="18.6328125" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="7.54296875" customWidth="1"/>
+    <col min="8" max="8" width="9.1796875" style="9" customWidth="1"/>
+    <col min="9" max="9" width="14.1796875" style="9" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="11.1796875" style="9" bestFit="1" customWidth="1"/>
+    <col min="11" max="11" width="14.1796875" style="9" bestFit="1" customWidth="1"/>
+    <col min="12" max="12" width="11.1796875" style="9" bestFit="1" customWidth="1"/>
+    <col min="13" max="16" width="9.1796875" style="9" customWidth="1"/>
+    <col min="17" max="17" width="9.7265625" style="9" bestFit="1" customWidth="1"/>
+    <col min="18" max="19" width="11.1796875" style="9" bestFit="1" customWidth="1"/>
+    <col min="20" max="20" width="9.1796875" style="9" customWidth="1"/>
+    <col min="21" max="21" width="14.1796875" style="9" bestFit="1" customWidth="1"/>
+    <col min="22" max="22" width="11.1796875" style="9" bestFit="1" customWidth="1"/>
+    <col min="23" max="23" width="14.1796875" style="9" bestFit="1" customWidth="1"/>
+    <col min="24" max="26" width="9.1796875" style="9" customWidth="1"/>
+    <col min="27" max="27" width="11.1796875" style="9" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:28" ht="35.25" customHeight="1" x14ac:dyDescent="0.95">
+    <row r="1" spans="1:28" ht="35.25" customHeight="1">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
     </row>
-    <row r="2" spans="1:28" ht="146" x14ac:dyDescent="0.5">
+    <row r="2" spans="1:28" ht="149.5">
       <c r="A2" s="2" t="s">
         <v>1</v>
       </c>
@@ -1248,7 +1244,7 @@
         <v>28</v>
       </c>
     </row>
-    <row r="3" spans="1:28" hidden="1" x14ac:dyDescent="0.5">
+    <row r="3" spans="1:28">
       <c r="A3" t="s">
         <v>29</v>
       </c>
@@ -1262,7 +1258,7 @@
         <v>31</v>
       </c>
       <c r="F3" t="s">
-        <v>163</v>
+        <v>161</v>
       </c>
       <c r="H3" s="9">
         <v>0.16500000000000001</v>
@@ -1294,7 +1290,7 @@
         <v>0.3</v>
       </c>
     </row>
-    <row r="4" spans="1:28" hidden="1" x14ac:dyDescent="0.5">
+    <row r="4" spans="1:28">
       <c r="A4" t="s">
         <v>29</v>
       </c>
@@ -1308,7 +1304,7 @@
         <v>32</v>
       </c>
       <c r="F4" t="s">
-        <v>131</v>
+        <v>129</v>
       </c>
       <c r="H4" s="9">
         <v>195</v>
@@ -1329,7 +1325,7 @@
         <v>270</v>
       </c>
     </row>
-    <row r="5" spans="1:28" hidden="1" x14ac:dyDescent="0.5">
+    <row r="5" spans="1:28">
       <c r="A5" t="s">
         <v>29</v>
       </c>
@@ -1343,7 +1339,7 @@
         <v>33</v>
       </c>
       <c r="F5" t="s">
-        <v>131</v>
+        <v>129</v>
       </c>
       <c r="I5" s="12"/>
       <c r="J5" s="12"/>
@@ -1351,7 +1347,7 @@
         <v>27.5</v>
       </c>
     </row>
-    <row r="6" spans="1:28" hidden="1" x14ac:dyDescent="0.5">
+    <row r="6" spans="1:28">
       <c r="A6" t="s">
         <v>29</v>
       </c>
@@ -1365,7 +1361,7 @@
         <v>34</v>
       </c>
       <c r="F6" t="s">
-        <v>158</v>
+        <v>156</v>
       </c>
       <c r="I6" s="12"/>
       <c r="J6" s="12"/>
@@ -1374,7 +1370,7 @@
         <v>0.22916666666666666</v>
       </c>
     </row>
-    <row r="7" spans="1:28" hidden="1" x14ac:dyDescent="0.5">
+    <row r="7" spans="1:28">
       <c r="A7" t="s">
         <v>29</v>
       </c>
@@ -1388,7 +1384,7 @@
         <v>35</v>
       </c>
       <c r="F7" t="s">
-        <v>164</v>
+        <v>162</v>
       </c>
       <c r="I7" s="12"/>
       <c r="J7" s="12"/>
@@ -1397,7 +1393,7 @@
         <v>0.9</v>
       </c>
     </row>
-    <row r="8" spans="1:28" hidden="1" x14ac:dyDescent="0.5">
+    <row r="8" spans="1:28">
       <c r="A8" t="s">
         <v>29</v>
       </c>
@@ -1411,7 +1407,7 @@
         <v>36</v>
       </c>
       <c r="F8" t="s">
-        <v>132</v>
+        <v>130</v>
       </c>
       <c r="H8" s="9">
         <v>0.9</v>
@@ -1435,7 +1431,7 @@
         <v>0.9</v>
       </c>
     </row>
-    <row r="9" spans="1:28" hidden="1" x14ac:dyDescent="0.5">
+    <row r="9" spans="1:28">
       <c r="A9" t="s">
         <v>29</v>
       </c>
@@ -1449,7 +1445,7 @@
         <v>38</v>
       </c>
       <c r="F9" t="s">
-        <v>140</v>
+        <v>138</v>
       </c>
       <c r="H9" s="9">
         <v>23</v>
@@ -1475,7 +1471,7 @@
         <v>28.4</v>
       </c>
     </row>
-    <row r="10" spans="1:28" x14ac:dyDescent="0.5">
+    <row r="10" spans="1:28">
       <c r="A10" t="s">
         <v>29</v>
       </c>
@@ -1519,7 +1515,7 @@
         <v>0.4</v>
       </c>
     </row>
-    <row r="11" spans="1:28" hidden="1" x14ac:dyDescent="0.5">
+    <row r="11" spans="1:28">
       <c r="A11" t="s">
         <v>29</v>
       </c>
@@ -1551,7 +1547,7 @@
         <v>0.9</v>
       </c>
     </row>
-    <row r="12" spans="1:28" hidden="1" x14ac:dyDescent="0.5">
+    <row r="12" spans="1:28">
       <c r="A12" t="s">
         <v>29</v>
       </c>
@@ -1565,7 +1561,7 @@
         <v>42</v>
       </c>
       <c r="F12" t="s">
-        <v>167</v>
+        <v>165</v>
       </c>
       <c r="H12" s="9">
         <f>54+60</f>
@@ -1594,7 +1590,7 @@
         <v>50</v>
       </c>
     </row>
-    <row r="13" spans="1:28" hidden="1" x14ac:dyDescent="0.5">
+    <row r="13" spans="1:28">
       <c r="A13" t="s">
         <v>29</v>
       </c>
@@ -1614,7 +1610,7 @@
         <v>0.15</v>
       </c>
     </row>
-    <row r="14" spans="1:28" hidden="1" x14ac:dyDescent="0.5">
+    <row r="14" spans="1:28">
       <c r="A14" t="s">
         <v>29</v>
       </c>
@@ -1657,7 +1653,7 @@
         <v>0.4</v>
       </c>
     </row>
-    <row r="15" spans="1:28" hidden="1" x14ac:dyDescent="0.5">
+    <row r="15" spans="1:28">
       <c r="A15" t="s">
         <v>29</v>
       </c>
@@ -1700,7 +1696,7 @@
         <v>0.6</v>
       </c>
     </row>
-    <row r="16" spans="1:28" hidden="1" x14ac:dyDescent="0.5">
+    <row r="16" spans="1:28">
       <c r="A16" t="s">
         <v>29</v>
       </c>
@@ -1714,7 +1710,7 @@
         <v>46</v>
       </c>
       <c r="F16" t="s">
-        <v>141</v>
+        <v>139</v>
       </c>
       <c r="H16" s="12">
         <v>26</v>
@@ -1740,7 +1736,7 @@
         <v>26</v>
       </c>
     </row>
-    <row r="17" spans="1:27" hidden="1" x14ac:dyDescent="0.5">
+    <row r="17" spans="1:27">
       <c r="A17" t="s">
         <v>29</v>
       </c>
@@ -1803,7 +1799,7 @@
         <v>0.08</v>
       </c>
     </row>
-    <row r="18" spans="1:27" hidden="1" x14ac:dyDescent="0.5">
+    <row r="18" spans="1:27">
       <c r="A18" t="s">
         <v>29</v>
       </c>
@@ -1851,7 +1847,7 @@
         <v>0.5</v>
       </c>
     </row>
-    <row r="19" spans="1:27" hidden="1" x14ac:dyDescent="0.5">
+    <row r="19" spans="1:27">
       <c r="A19" t="s">
         <v>29</v>
       </c>
@@ -1895,7 +1891,7 @@
         <v>100000</v>
       </c>
     </row>
-    <row r="20" spans="1:27" hidden="1" x14ac:dyDescent="0.5">
+    <row r="20" spans="1:27">
       <c r="A20" t="s">
         <v>29</v>
       </c>
@@ -1932,7 +1928,7 @@
         <v>0.3</v>
       </c>
     </row>
-    <row r="21" spans="1:27" hidden="1" x14ac:dyDescent="0.5">
+    <row r="21" spans="1:27">
       <c r="A21" t="s">
         <v>29</v>
       </c>
@@ -1946,7 +1942,7 @@
         <v>51</v>
       </c>
       <c r="F21" t="s">
-        <v>163</v>
+        <v>161</v>
       </c>
       <c r="I21" s="12"/>
       <c r="J21" s="12"/>
@@ -1968,7 +1964,7 @@
         <v>1.23</v>
       </c>
     </row>
-    <row r="22" spans="1:27" hidden="1" x14ac:dyDescent="0.5">
+    <row r="22" spans="1:27">
       <c r="A22" t="s">
         <v>29</v>
       </c>
@@ -1992,7 +1988,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="23" spans="1:27" hidden="1" x14ac:dyDescent="0.5">
+    <row r="23" spans="1:27">
       <c r="A23" t="s">
         <v>29</v>
       </c>
@@ -2006,7 +2002,7 @@
         <v>53</v>
       </c>
       <c r="F23" t="s">
-        <v>142</v>
+        <v>140</v>
       </c>
       <c r="I23" s="12"/>
       <c r="J23" s="12"/>
@@ -2031,7 +2027,7 @@
         <v>2.69</v>
       </c>
     </row>
-    <row r="24" spans="1:27" hidden="1" x14ac:dyDescent="0.5">
+    <row r="24" spans="1:27">
       <c r="A24" t="s">
         <v>29</v>
       </c>
@@ -2055,7 +2051,7 @@
         <v>0.88</v>
       </c>
     </row>
-    <row r="25" spans="1:27" hidden="1" x14ac:dyDescent="0.5">
+    <row r="25" spans="1:27">
       <c r="A25" t="s">
         <v>29</v>
       </c>
@@ -2108,7 +2104,7 @@
         <v>0.86206896551724133</v>
       </c>
     </row>
-    <row r="26" spans="1:27" hidden="1" x14ac:dyDescent="0.5">
+    <row r="26" spans="1:27">
       <c r="A26" t="s">
         <v>29</v>
       </c>
@@ -2122,7 +2118,7 @@
         <v>57</v>
       </c>
       <c r="F26" t="s">
-        <v>157</v>
+        <v>155</v>
       </c>
       <c r="I26" s="12"/>
       <c r="J26" s="12"/>
@@ -2137,7 +2133,7 @@
         <v>63</v>
       </c>
     </row>
-    <row r="27" spans="1:27" hidden="1" x14ac:dyDescent="0.5">
+    <row r="27" spans="1:27">
       <c r="A27" t="s">
         <v>29</v>
       </c>
@@ -2165,7 +2161,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="28" spans="1:27" hidden="1" x14ac:dyDescent="0.5">
+    <row r="28" spans="1:27">
       <c r="A28" t="s">
         <v>29</v>
       </c>
@@ -2193,7 +2189,7 @@
         <v>0.97</v>
       </c>
     </row>
-    <row r="29" spans="1:27" hidden="1" x14ac:dyDescent="0.5">
+    <row r="29" spans="1:27">
       <c r="A29" t="s">
         <v>29</v>
       </c>
@@ -2207,7 +2203,7 @@
         <v>60</v>
       </c>
       <c r="F29" t="s">
-        <v>143</v>
+        <v>141</v>
       </c>
       <c r="I29" s="12"/>
       <c r="J29" s="12"/>
@@ -2219,7 +2215,7 @@
         <v>12.15</v>
       </c>
     </row>
-    <row r="30" spans="1:27" hidden="1" x14ac:dyDescent="0.5">
+    <row r="30" spans="1:27">
       <c r="A30" t="s">
         <v>29</v>
       </c>
@@ -2233,7 +2229,7 @@
         <v>61</v>
       </c>
       <c r="F30" t="s">
-        <v>152</v>
+        <v>150</v>
       </c>
       <c r="I30" s="12"/>
       <c r="J30" s="12"/>
@@ -2241,7 +2237,7 @@
       <c r="L30" s="12"/>
       <c r="M30" s="11"/>
     </row>
-    <row r="31" spans="1:27" hidden="1" x14ac:dyDescent="0.5">
+    <row r="31" spans="1:27">
       <c r="A31" t="s">
         <v>29</v>
       </c>
@@ -2255,7 +2251,7 @@
         <v>62</v>
       </c>
       <c r="F31" s="5" t="s">
-        <v>141</v>
+        <v>139</v>
       </c>
       <c r="I31" s="12"/>
       <c r="J31" s="12"/>
@@ -2269,7 +2265,7 @@
         <v>120</v>
       </c>
     </row>
-    <row r="32" spans="1:27" hidden="1" x14ac:dyDescent="0.5">
+    <row r="32" spans="1:27">
       <c r="A32" t="s">
         <v>29</v>
       </c>
@@ -2283,7 +2279,7 @@
         <v>63</v>
       </c>
       <c r="F32" s="5" t="s">
-        <v>141</v>
+        <v>139</v>
       </c>
       <c r="I32" s="12"/>
       <c r="J32" s="12"/>
@@ -2297,7 +2293,7 @@
         <v>47.1</v>
       </c>
     </row>
-    <row r="33" spans="1:27" hidden="1" x14ac:dyDescent="0.5">
+    <row r="33" spans="1:27">
       <c r="A33" t="s">
         <v>29</v>
       </c>
@@ -2311,7 +2307,7 @@
         <v>64</v>
       </c>
       <c r="F33" s="4" t="s">
-        <v>159</v>
+        <v>157</v>
       </c>
       <c r="I33" s="12"/>
       <c r="J33" s="12"/>
@@ -2322,7 +2318,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="34" spans="1:27" hidden="1" x14ac:dyDescent="0.5">
+    <row r="34" spans="1:27">
       <c r="A34" t="s">
         <v>29</v>
       </c>
@@ -2347,7 +2343,7 @@
         <v>0.97</v>
       </c>
     </row>
-    <row r="35" spans="1:27" hidden="1" x14ac:dyDescent="0.5">
+    <row r="35" spans="1:27">
       <c r="A35" t="s">
         <v>29</v>
       </c>
@@ -2373,7 +2369,7 @@
       </c>
       <c r="Q35" s="12"/>
     </row>
-    <row r="36" spans="1:27" hidden="1" x14ac:dyDescent="0.5">
+    <row r="36" spans="1:27">
       <c r="A36" t="s">
         <v>29</v>
       </c>
@@ -2406,7 +2402,7 @@
         <v>700</v>
       </c>
     </row>
-    <row r="37" spans="1:27" hidden="1" x14ac:dyDescent="0.5">
+    <row r="37" spans="1:27">
       <c r="A37" t="s">
         <v>29</v>
       </c>
@@ -2420,7 +2416,7 @@
         <v>69</v>
       </c>
       <c r="F37" s="4" t="s">
-        <v>142</v>
+        <v>140</v>
       </c>
       <c r="I37" s="12"/>
       <c r="J37" s="12"/>
@@ -2439,7 +2435,7 @@
         <v>2000</v>
       </c>
     </row>
-    <row r="38" spans="1:27" hidden="1" x14ac:dyDescent="0.5">
+    <row r="38" spans="1:27">
       <c r="A38" t="s">
         <v>29</v>
       </c>
@@ -2450,7 +2446,7 @@
         <v>30</v>
       </c>
       <c r="D38" t="s">
-        <v>171</v>
+        <v>169</v>
       </c>
       <c r="F38" s="4" t="s">
         <v>40</v>
@@ -2471,7 +2467,7 @@
         <v>0.97</v>
       </c>
     </row>
-    <row r="39" spans="1:27" hidden="1" x14ac:dyDescent="0.5">
+    <row r="39" spans="1:27">
       <c r="A39" t="s">
         <v>29</v>
       </c>
@@ -2482,10 +2478,10 @@
         <v>37</v>
       </c>
       <c r="D39" t="s">
-        <v>173</v>
+        <v>171</v>
       </c>
       <c r="F39" s="4" t="s">
-        <v>168</v>
+        <v>166</v>
       </c>
       <c r="I39" s="12"/>
       <c r="J39" s="12"/>
@@ -2505,7 +2501,7 @@
         <v>0.45</v>
       </c>
     </row>
-    <row r="40" spans="1:27" hidden="1" x14ac:dyDescent="0.5">
+    <row r="40" spans="1:27">
       <c r="A40" t="s">
         <v>29</v>
       </c>
@@ -2516,10 +2512,10 @@
         <v>37</v>
       </c>
       <c r="D40" t="s">
-        <v>174</v>
+        <v>172</v>
       </c>
       <c r="F40" s="4" t="s">
-        <v>168</v>
+        <v>166</v>
       </c>
       <c r="I40" s="12"/>
       <c r="J40" s="12"/>
@@ -2539,7 +2535,7 @@
         <v>0.82</v>
       </c>
     </row>
-    <row r="41" spans="1:27" hidden="1" x14ac:dyDescent="0.5">
+    <row r="41" spans="1:27">
       <c r="A41" t="s">
         <v>29</v>
       </c>
@@ -2550,10 +2546,10 @@
         <v>37</v>
       </c>
       <c r="D41" t="s">
-        <v>175</v>
+        <v>173</v>
       </c>
       <c r="F41" s="4" t="s">
-        <v>144</v>
+        <v>142</v>
       </c>
       <c r="I41" s="12"/>
       <c r="J41" s="12"/>
@@ -2574,7 +2570,7 @@
         <v>0.24709042076991944</v>
       </c>
     </row>
-    <row r="42" spans="1:27" ht="11.5" hidden="1" customHeight="1" x14ac:dyDescent="0.5">
+    <row r="42" spans="1:27" ht="11.5" customHeight="1">
       <c r="A42" t="s">
         <v>2</v>
       </c>
@@ -2592,7 +2588,7 @@
         <v>Met coal</v>
       </c>
       <c r="F42" t="s">
-        <v>133</v>
+        <v>131</v>
       </c>
       <c r="H42" s="12">
         <v>1.2849999999999999</v>
@@ -2640,7 +2636,7 @@
         <v>1.2849999999999999</v>
       </c>
     </row>
-    <row r="43" spans="1:27" hidden="1" x14ac:dyDescent="0.5">
+    <row r="43" spans="1:27">
       <c r="A43" t="s">
         <v>2</v>
       </c>
@@ -2658,7 +2654,7 @@
         <v>COG</v>
       </c>
       <c r="F43" t="s">
-        <v>145</v>
+        <v>143</v>
       </c>
       <c r="H43" s="12">
         <f>3.3*H14</f>
@@ -2707,7 +2703,7 @@
         <v>2.9699999999999998</v>
       </c>
     </row>
-    <row r="44" spans="1:27" hidden="1" x14ac:dyDescent="0.5">
+    <row r="44" spans="1:27">
       <c r="A44" t="s">
         <v>2</v>
       </c>
@@ -2725,7 +2721,7 @@
         <v>BF gas</v>
       </c>
       <c r="F44" t="s">
-        <v>145</v>
+        <v>143</v>
       </c>
       <c r="H44" s="12">
         <f>3.3-H43</f>
@@ -2770,7 +2766,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="45" spans="1:27" hidden="1" x14ac:dyDescent="0.5">
+    <row r="45" spans="1:27">
       <c r="A45" t="s">
         <v>2</v>
       </c>
@@ -2788,7 +2784,7 @@
         <v>Electricity</v>
       </c>
       <c r="F45" t="s">
-        <v>145</v>
+        <v>143</v>
       </c>
       <c r="H45" s="12">
         <v>0.125</v>
@@ -2836,7 +2832,7 @@
         <v>0.125</v>
       </c>
     </row>
-    <row r="46" spans="1:27" hidden="1" x14ac:dyDescent="0.5">
+    <row r="46" spans="1:27">
       <c r="A46" t="s">
         <v>2</v>
       </c>
@@ -2854,7 +2850,7 @@
         <v>Steam</v>
       </c>
       <c r="F46" t="s">
-        <v>145</v>
+        <v>143</v>
       </c>
       <c r="H46" s="12">
         <v>0.42</v>
@@ -2902,7 +2898,7 @@
         <v>0.378</v>
       </c>
     </row>
-    <row r="47" spans="1:27" hidden="1" x14ac:dyDescent="0.5">
+    <row r="47" spans="1:27">
       <c r="A47" t="s">
         <v>2</v>
       </c>
@@ -2920,7 +2916,7 @@
         <v>Iron ore</v>
       </c>
       <c r="F47" t="s">
-        <v>134</v>
+        <v>132</v>
       </c>
       <c r="H47" s="12">
         <f>0.81/(62%/67%)</f>
@@ -2969,7 +2965,7 @@
         <v>0.87532258064516144</v>
       </c>
     </row>
-    <row r="48" spans="1:27" hidden="1" x14ac:dyDescent="0.5">
+    <row r="48" spans="1:27">
       <c r="A48" t="s">
         <v>2</v>
       </c>
@@ -2987,7 +2983,7 @@
         <v>Thermal coal</v>
       </c>
       <c r="F48" t="s">
-        <v>146</v>
+        <v>144</v>
       </c>
       <c r="H48" s="12">
         <f>1.277</f>
@@ -3036,7 +3032,7 @@
         <v>1.1493</v>
       </c>
     </row>
-    <row r="49" spans="1:27" hidden="1" x14ac:dyDescent="0.5">
+    <row r="49" spans="1:27">
       <c r="A49" t="s">
         <v>2</v>
       </c>
@@ -3054,7 +3050,7 @@
         <v>COG</v>
       </c>
       <c r="F49" t="s">
-        <v>146</v>
+        <v>144</v>
       </c>
       <c r="H49" s="12">
         <f>0.67*$H$14</f>
@@ -3103,7 +3099,7 @@
         <v>0.60299999999999998</v>
       </c>
     </row>
-    <row r="50" spans="1:27" hidden="1" x14ac:dyDescent="0.5">
+    <row r="50" spans="1:27">
       <c r="A50" t="s">
         <v>2</v>
       </c>
@@ -3121,7 +3117,7 @@
         <v>BF gas</v>
       </c>
       <c r="F50" t="s">
-        <v>146</v>
+        <v>144</v>
       </c>
       <c r="H50" s="12">
         <f>(0.67-H49)</f>
@@ -3166,7 +3162,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="51" spans="1:27" hidden="1" x14ac:dyDescent="0.5">
+    <row r="51" spans="1:27">
       <c r="A51" t="s">
         <v>2</v>
       </c>
@@ -3184,7 +3180,7 @@
         <v>Electricity</v>
       </c>
       <c r="F51" t="s">
-        <v>146</v>
+        <v>144</v>
       </c>
       <c r="H51" s="12">
         <f>0.04</f>
@@ -3233,7 +3229,7 @@
         <v>0.04</v>
       </c>
     </row>
-    <row r="52" spans="1:27" hidden="1" x14ac:dyDescent="0.5">
+    <row r="52" spans="1:27">
       <c r="A52" t="s">
         <v>2</v>
       </c>
@@ -3251,7 +3247,7 @@
         <v>Iron ore</v>
       </c>
       <c r="F52" t="s">
-        <v>135</v>
+        <v>133</v>
       </c>
       <c r="H52" s="12">
         <f>0.95/(62%/67%)</f>
@@ -3317,7 +3313,7 @@
         <v>1.0266129032258065</v>
       </c>
     </row>
-    <row r="53" spans="1:27" hidden="1" x14ac:dyDescent="0.5">
+    <row r="53" spans="1:27">
       <c r="A53" t="s">
         <v>2</v>
       </c>
@@ -3335,7 +3331,7 @@
         <v>COG</v>
       </c>
       <c r="F53" t="s">
-        <v>147</v>
+        <v>145</v>
       </c>
       <c r="H53" s="12">
         <f>0.31*$H$14</f>
@@ -3398,7 +3394,7 @@
         <v>0.27900000000000003</v>
       </c>
     </row>
-    <row r="54" spans="1:27" hidden="1" x14ac:dyDescent="0.5">
+    <row r="54" spans="1:27">
       <c r="A54" t="s">
         <v>2</v>
       </c>
@@ -3416,7 +3412,7 @@
         <v>BF gas</v>
       </c>
       <c r="F54" t="s">
-        <v>147</v>
+        <v>145</v>
       </c>
       <c r="H54" s="12">
         <f>0.31-H53</f>
@@ -3475,7 +3471,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="55" spans="1:27" hidden="1" x14ac:dyDescent="0.5">
+    <row r="55" spans="1:27">
       <c r="A55" t="s">
         <v>2</v>
       </c>
@@ -3493,7 +3489,7 @@
         <v>Natural gas</v>
       </c>
       <c r="F55" t="s">
-        <v>147</v>
+        <v>145</v>
       </c>
       <c r="H55" s="12">
         <v>0.01</v>
@@ -3557,7 +3553,7 @@
         <v>9.0000000000000011E-3</v>
       </c>
     </row>
-    <row r="56" spans="1:27" hidden="1" x14ac:dyDescent="0.5">
+    <row r="56" spans="1:27">
       <c r="A56" t="s">
         <v>2</v>
       </c>
@@ -3575,7 +3571,7 @@
         <v>Thermal coal</v>
       </c>
       <c r="F56" t="s">
-        <v>147</v>
+        <v>145</v>
       </c>
       <c r="H56" s="12">
         <v>0.34</v>
@@ -3633,7 +3629,7 @@
         <v>0.30600000000000005</v>
       </c>
     </row>
-    <row r="57" spans="1:27" hidden="1" x14ac:dyDescent="0.5">
+    <row r="57" spans="1:27">
       <c r="A57" t="s">
         <v>2</v>
       </c>
@@ -3648,7 +3644,7 @@
       </c>
       <c r="E57" s="7"/>
       <c r="F57" t="s">
-        <v>147</v>
+        <v>145</v>
       </c>
       <c r="H57" s="12"/>
       <c r="J57" s="12"/>
@@ -3686,7 +3682,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="58" spans="1:27" hidden="1" x14ac:dyDescent="0.5">
+    <row r="58" spans="1:27">
       <c r="A58" t="s">
         <v>2</v>
       </c>
@@ -3704,7 +3700,7 @@
         <v>Electricity</v>
       </c>
       <c r="F58" t="s">
-        <v>147</v>
+        <v>145</v>
       </c>
       <c r="H58" s="12">
         <v>7.5999999999999998E-2</v>
@@ -3769,7 +3765,7 @@
         <v>7.5999999999999998E-2</v>
       </c>
     </row>
-    <row r="59" spans="1:27" hidden="1" x14ac:dyDescent="0.5">
+    <row r="59" spans="1:27">
       <c r="A59" t="s">
         <v>2</v>
       </c>
@@ -3780,14 +3776,14 @@
         <v>73</v>
       </c>
       <c r="D59" t="s">
-        <v>84</v>
+        <v>106</v>
       </c>
       <c r="E59" t="str">
         <f t="shared" si="0"/>
-        <v xml:space="preserve">Biomethane </v>
+        <v>Biomethane</v>
       </c>
       <c r="F59" t="s">
-        <v>147</v>
+        <v>145</v>
       </c>
       <c r="H59" s="12"/>
       <c r="J59" s="12"/>
@@ -3808,22 +3804,22 @@
         <v>0</v>
       </c>
     </row>
-    <row r="60" spans="1:27" hidden="1" x14ac:dyDescent="0.5">
+    <row r="60" spans="1:27">
       <c r="A60" t="s">
         <v>2</v>
       </c>
       <c r="B60" t="s">
-        <v>85</v>
+        <v>84</v>
       </c>
       <c r="C60" t="s">
         <v>71</v>
       </c>
       <c r="D60" t="s">
-        <v>86</v>
+        <v>85</v>
       </c>
       <c r="E60" s="7"/>
       <c r="F60" t="s">
-        <v>136</v>
+        <v>134</v>
       </c>
       <c r="H60" s="12">
         <v>0.99199999999999999</v>
@@ -3856,12 +3852,12 @@
         <v>0.99199999999999999</v>
       </c>
     </row>
-    <row r="61" spans="1:27" hidden="1" x14ac:dyDescent="0.5">
+    <row r="61" spans="1:27">
       <c r="A61" t="s">
         <v>2</v>
       </c>
       <c r="B61" t="s">
-        <v>85</v>
+        <v>84</v>
       </c>
       <c r="C61" t="s">
         <v>71</v>
@@ -3874,7 +3870,7 @@
         <v>Iron ore</v>
       </c>
       <c r="F61" t="s">
-        <v>136</v>
+        <v>134</v>
       </c>
       <c r="H61" s="12">
         <v>0.15</v>
@@ -3907,22 +3903,22 @@
         <v>0.15</v>
       </c>
     </row>
-    <row r="62" spans="1:27" hidden="1" x14ac:dyDescent="0.5">
+    <row r="62" spans="1:27">
       <c r="A62" t="s">
         <v>2</v>
       </c>
       <c r="B62" t="s">
-        <v>85</v>
+        <v>84</v>
       </c>
       <c r="C62" t="s">
         <v>71</v>
       </c>
       <c r="D62" t="s">
-        <v>87</v>
+        <v>86</v>
       </c>
       <c r="E62" s="7"/>
       <c r="F62" t="s">
-        <v>136</v>
+        <v>134</v>
       </c>
       <c r="H62" s="12">
         <v>0.435</v>
@@ -3955,25 +3951,25 @@
         <v>0.435</v>
       </c>
     </row>
-    <row r="63" spans="1:27" hidden="1" x14ac:dyDescent="0.5">
+    <row r="63" spans="1:27">
       <c r="A63" t="s">
         <v>2</v>
       </c>
       <c r="B63" t="s">
-        <v>85</v>
+        <v>84</v>
       </c>
       <c r="C63" t="s">
         <v>71</v>
       </c>
       <c r="D63" t="s">
-        <v>88</v>
+        <v>87</v>
       </c>
       <c r="E63" t="str">
         <f t="shared" si="0"/>
         <v>Coke</v>
       </c>
       <c r="F63" t="s">
-        <v>136</v>
+        <v>134</v>
       </c>
       <c r="H63" s="12">
         <f>0.482-H67*$H$8/1000</f>
@@ -4007,25 +4003,25 @@
         <v>0.21509999999999999</v>
       </c>
     </row>
-    <row r="64" spans="1:27" hidden="1" x14ac:dyDescent="0.5">
+    <row r="64" spans="1:27">
       <c r="A64" t="s">
         <v>2</v>
       </c>
       <c r="B64" t="s">
-        <v>85</v>
+        <v>84</v>
       </c>
       <c r="C64" t="s">
         <v>71</v>
       </c>
       <c r="D64" t="s">
-        <v>89</v>
+        <v>88</v>
       </c>
       <c r="E64" t="str">
         <f t="shared" si="0"/>
         <v>DRI</v>
       </c>
       <c r="F64" t="s">
-        <v>136</v>
+        <v>134</v>
       </c>
       <c r="H64" s="12">
         <v>0</v>
@@ -4049,25 +4045,25 @@
         <v>0</v>
       </c>
     </row>
-    <row r="65" spans="1:27" hidden="1" x14ac:dyDescent="0.5">
+    <row r="65" spans="1:27">
       <c r="A65" t="s">
         <v>2</v>
       </c>
       <c r="B65" t="s">
-        <v>85</v>
+        <v>84</v>
       </c>
       <c r="C65" t="s">
         <v>71</v>
       </c>
       <c r="D65" t="s">
-        <v>90</v>
+        <v>89</v>
       </c>
       <c r="E65" t="str">
         <f t="shared" si="0"/>
         <v>Biomass</v>
       </c>
       <c r="F65" t="s">
-        <v>148</v>
+        <v>146</v>
       </c>
       <c r="H65" s="12"/>
       <c r="I65" s="12"/>
@@ -4080,25 +4076,25 @@
         <v>0.67876000000000003</v>
       </c>
     </row>
-    <row r="66" spans="1:27" hidden="1" x14ac:dyDescent="0.5">
+    <row r="66" spans="1:27">
       <c r="A66" t="s">
         <v>2</v>
       </c>
       <c r="B66" t="s">
-        <v>85</v>
+        <v>84</v>
       </c>
       <c r="C66" t="s">
+        <v>90</v>
+      </c>
+      <c r="D66" t="s">
         <v>91</v>
-      </c>
-      <c r="D66" t="s">
-        <v>92</v>
       </c>
       <c r="E66" t="str">
         <f t="shared" si="0"/>
         <v>Hydrogen</v>
       </c>
       <c r="F66" t="s">
-        <v>155</v>
+        <v>153</v>
       </c>
       <c r="H66" s="12"/>
       <c r="I66" s="12"/>
@@ -4115,15 +4111,15 @@
         <v>0</v>
       </c>
     </row>
-    <row r="67" spans="1:27" hidden="1" x14ac:dyDescent="0.5">
+    <row r="67" spans="1:27">
       <c r="A67" t="s">
         <v>2</v>
       </c>
       <c r="B67" t="s">
-        <v>85</v>
+        <v>84</v>
       </c>
       <c r="C67" t="s">
-        <v>91</v>
+        <v>90</v>
       </c>
       <c r="D67" t="s">
         <v>80</v>
@@ -4133,7 +4129,7 @@
         <v>Thermal coal</v>
       </c>
       <c r="F67" t="s">
-        <v>155</v>
+        <v>153</v>
       </c>
       <c r="H67" s="12">
         <f>H4</f>
@@ -4156,25 +4152,25 @@
         <v>0</v>
       </c>
     </row>
-    <row r="68" spans="1:27" hidden="1" x14ac:dyDescent="0.5">
+    <row r="68" spans="1:27">
       <c r="A68" t="s">
         <v>2</v>
       </c>
       <c r="B68" t="s">
-        <v>85</v>
+        <v>84</v>
       </c>
       <c r="C68" t="s">
-        <v>91</v>
+        <v>90</v>
       </c>
       <c r="D68" t="s">
-        <v>90</v>
+        <v>89</v>
       </c>
       <c r="E68" t="str">
         <f t="shared" si="0"/>
         <v>Biomass</v>
       </c>
       <c r="F68" t="s">
-        <v>155</v>
+        <v>153</v>
       </c>
       <c r="J68" s="12">
         <f>J4</f>
@@ -4192,25 +4188,25 @@
         <v>270</v>
       </c>
     </row>
-    <row r="69" spans="1:27" hidden="1" x14ac:dyDescent="0.5">
+    <row r="69" spans="1:27">
       <c r="A69" t="s">
         <v>2</v>
       </c>
       <c r="B69" t="s">
-        <v>85</v>
+        <v>84</v>
       </c>
       <c r="C69" t="s">
-        <v>91</v>
+        <v>90</v>
       </c>
       <c r="D69" t="s">
-        <v>172</v>
+        <v>170</v>
       </c>
       <c r="E69" t="str">
         <f t="shared" si="0"/>
         <v>Plastic waste</v>
       </c>
       <c r="F69" t="s">
-        <v>155</v>
+        <v>153</v>
       </c>
       <c r="J69" s="12"/>
       <c r="L69" s="12"/>
@@ -4220,15 +4216,15 @@
         <v>230</v>
       </c>
     </row>
-    <row r="70" spans="1:27" hidden="1" x14ac:dyDescent="0.5">
+    <row r="70" spans="1:27">
       <c r="A70" t="s">
         <v>2</v>
       </c>
       <c r="B70" t="s">
-        <v>85</v>
+        <v>84</v>
       </c>
       <c r="C70" t="s">
-        <v>93</v>
+        <v>92</v>
       </c>
       <c r="D70" t="s">
         <v>75</v>
@@ -4238,7 +4234,7 @@
         <v>BF gas</v>
       </c>
       <c r="F70" t="s">
-        <v>148</v>
+        <v>146</v>
       </c>
       <c r="H70" s="12">
         <v>2.2000000000000002</v>
@@ -4267,15 +4263,15 @@
         <v>3.2261039999999999</v>
       </c>
     </row>
-    <row r="71" spans="1:27" hidden="1" x14ac:dyDescent="0.5">
+    <row r="71" spans="1:27">
       <c r="A71" t="s">
         <v>2</v>
       </c>
       <c r="B71" t="s">
-        <v>85</v>
+        <v>84</v>
       </c>
       <c r="C71" t="s">
-        <v>93</v>
+        <v>92</v>
       </c>
       <c r="D71" t="s">
         <v>74</v>
@@ -4285,7 +4281,7 @@
         <v>COG</v>
       </c>
       <c r="F71" t="s">
-        <v>148</v>
+        <v>146</v>
       </c>
       <c r="H71" s="12">
         <v>0.32</v>
@@ -4317,15 +4313,15 @@
         <v>0.8</v>
       </c>
     </row>
-    <row r="72" spans="1:27" hidden="1" x14ac:dyDescent="0.5">
+    <row r="72" spans="1:27">
       <c r="A72" t="s">
         <v>2</v>
       </c>
       <c r="B72" t="s">
-        <v>85</v>
+        <v>84</v>
       </c>
       <c r="C72" t="s">
-        <v>93</v>
+        <v>92</v>
       </c>
       <c r="D72" t="s">
         <v>82</v>
@@ -4335,7 +4331,7 @@
         <v>Natural gas</v>
       </c>
       <c r="F72" t="s">
-        <v>148</v>
+        <v>146</v>
       </c>
       <c r="H72" s="12">
         <v>0.25</v>
@@ -4372,25 +4368,25 @@
         <v>0.22500000000000001</v>
       </c>
     </row>
-    <row r="73" spans="1:27" hidden="1" x14ac:dyDescent="0.5">
+    <row r="73" spans="1:27">
       <c r="A73" t="s">
         <v>2</v>
       </c>
       <c r="B73" t="s">
-        <v>85</v>
+        <v>84</v>
       </c>
       <c r="C73" t="s">
+        <v>92</v>
+      </c>
+      <c r="D73" t="s">
         <v>93</v>
-      </c>
-      <c r="D73" t="s">
-        <v>94</v>
       </c>
       <c r="E73" t="str">
         <f t="shared" si="0"/>
         <v>BOF gas</v>
       </c>
       <c r="F73" t="s">
-        <v>148</v>
+        <v>146</v>
       </c>
       <c r="H73" s="12">
         <v>0.35</v>
@@ -4423,15 +4419,15 @@
         <v>0.315</v>
       </c>
     </row>
-    <row r="74" spans="1:27" hidden="1" x14ac:dyDescent="0.5">
+    <row r="74" spans="1:27">
       <c r="A74" t="s">
         <v>2</v>
       </c>
       <c r="B74" t="s">
-        <v>85</v>
+        <v>84</v>
       </c>
       <c r="C74" t="s">
-        <v>95</v>
+        <v>94</v>
       </c>
       <c r="D74" t="s">
         <v>76</v>
@@ -4441,7 +4437,7 @@
         <v>Electricity</v>
       </c>
       <c r="F74" t="s">
-        <v>148</v>
+        <v>146</v>
       </c>
       <c r="H74" s="12">
         <v>0.26800000000000002</v>
@@ -4474,15 +4470,15 @@
         <v>0.26800000000000002</v>
       </c>
     </row>
-    <row r="75" spans="1:27" hidden="1" x14ac:dyDescent="0.5">
+    <row r="75" spans="1:27">
       <c r="A75" t="s">
         <v>2</v>
       </c>
       <c r="B75" t="s">
-        <v>85</v>
+        <v>84</v>
       </c>
       <c r="C75" t="s">
-        <v>96</v>
+        <v>95</v>
       </c>
       <c r="D75" t="s">
         <v>77</v>
@@ -4492,7 +4488,7 @@
         <v>Steam</v>
       </c>
       <c r="F75" t="s">
-        <v>148</v>
+        <v>146</v>
       </c>
       <c r="H75" s="12">
         <v>4.8000000000000001E-2</v>
@@ -4525,25 +4521,25 @@
         <v>4.3200000000000002E-2</v>
       </c>
     </row>
-    <row r="76" spans="1:27" hidden="1" x14ac:dyDescent="0.5">
+    <row r="76" spans="1:27">
       <c r="A76" t="s">
         <v>2</v>
       </c>
       <c r="B76" t="s">
-        <v>85</v>
+        <v>84</v>
       </c>
       <c r="C76" t="s">
+        <v>95</v>
+      </c>
+      <c r="D76" t="s">
         <v>96</v>
-      </c>
-      <c r="D76" t="s">
-        <v>97</v>
       </c>
       <c r="E76" t="str">
         <f t="shared" si="0"/>
         <v>BF slag</v>
       </c>
       <c r="F76" t="s">
-        <v>155</v>
+        <v>153</v>
       </c>
       <c r="H76" s="12">
         <v>330</v>
@@ -4576,15 +4572,15 @@
         <v>330</v>
       </c>
     </row>
-    <row r="77" spans="1:27" hidden="1" x14ac:dyDescent="0.5">
+    <row r="77" spans="1:27">
       <c r="A77" t="s">
         <v>2</v>
       </c>
       <c r="B77" t="s">
-        <v>98</v>
+        <v>97</v>
       </c>
       <c r="C77" t="s">
-        <v>96</v>
+        <v>95</v>
       </c>
       <c r="D77" t="s">
         <v>76</v>
@@ -4594,7 +4590,7 @@
         <v>Electricity</v>
       </c>
       <c r="F77" t="s">
-        <v>142</v>
+        <v>140</v>
       </c>
       <c r="H77" s="9">
         <f>H12*G136*3.6/1000</f>
@@ -4645,22 +4641,22 @@
         <v>0.19397557124088433</v>
       </c>
     </row>
-    <row r="78" spans="1:27" hidden="1" x14ac:dyDescent="0.5">
+    <row r="78" spans="1:27">
       <c r="A78" t="s">
         <v>2</v>
       </c>
       <c r="B78" t="s">
-        <v>99</v>
+        <v>98</v>
       </c>
       <c r="C78" t="s">
         <v>71</v>
       </c>
       <c r="D78" t="s">
-        <v>100</v>
+        <v>99</v>
       </c>
       <c r="E78" s="7"/>
       <c r="F78" t="s">
-        <v>137</v>
+        <v>135</v>
       </c>
       <c r="H78" s="12">
         <f>(1+$H$17)-H79</f>
@@ -4711,25 +4707,25 @@
         <v>0.78</v>
       </c>
     </row>
-    <row r="79" spans="1:27" hidden="1" x14ac:dyDescent="0.5">
+    <row r="79" spans="1:27">
       <c r="A79" t="s">
         <v>2</v>
       </c>
       <c r="B79" t="s">
-        <v>99</v>
+        <v>98</v>
       </c>
       <c r="C79" t="s">
         <v>71</v>
       </c>
       <c r="D79" t="s">
-        <v>101</v>
+        <v>100</v>
       </c>
       <c r="E79" t="str">
         <f t="shared" si="0"/>
         <v>Scrap</v>
       </c>
       <c r="F79" t="s">
-        <v>137</v>
+        <v>135</v>
       </c>
       <c r="H79" s="12">
         <f>H3</f>
@@ -4768,15 +4764,15 @@
         <v>0.3</v>
       </c>
     </row>
-    <row r="80" spans="1:27" hidden="1" x14ac:dyDescent="0.5">
+    <row r="80" spans="1:27">
       <c r="A80" t="s">
         <v>2</v>
       </c>
       <c r="B80" t="s">
-        <v>99</v>
+        <v>98</v>
       </c>
       <c r="C80" t="s">
-        <v>102</v>
+        <v>101</v>
       </c>
       <c r="D80" t="s">
         <v>82</v>
@@ -4786,7 +4782,7 @@
         <v>Natural gas</v>
       </c>
       <c r="F80" t="s">
-        <v>142</v>
+        <v>140</v>
       </c>
       <c r="H80" s="12">
         <v>0.04</v>
@@ -4823,15 +4819,15 @@
         <v>3.6000000000000004E-2</v>
       </c>
     </row>
-    <row r="81" spans="1:27" hidden="1" x14ac:dyDescent="0.5">
+    <row r="81" spans="1:27">
       <c r="A81" t="s">
         <v>2</v>
       </c>
       <c r="B81" t="s">
-        <v>99</v>
+        <v>98</v>
       </c>
       <c r="C81" t="s">
-        <v>102</v>
+        <v>101</v>
       </c>
       <c r="D81" t="s">
         <v>74</v>
@@ -4841,7 +4837,7 @@
         <v>COG</v>
       </c>
       <c r="F81" t="s">
-        <v>142</v>
+        <v>140</v>
       </c>
       <c r="H81" s="12">
         <v>0.01</v>
@@ -4871,15 +4867,15 @@
         <v>9.0000000000000011E-3</v>
       </c>
     </row>
-    <row r="82" spans="1:27" hidden="1" x14ac:dyDescent="0.5">
+    <row r="82" spans="1:27">
       <c r="A82" t="s">
         <v>2</v>
       </c>
       <c r="B82" t="s">
-        <v>99</v>
+        <v>98</v>
       </c>
       <c r="C82" t="s">
-        <v>102</v>
+        <v>101</v>
       </c>
       <c r="D82" t="s">
         <v>75</v>
@@ -4889,7 +4885,7 @@
         <v>BF gas</v>
       </c>
       <c r="F82" t="s">
-        <v>142</v>
+        <v>140</v>
       </c>
       <c r="H82" s="12">
         <v>0.03</v>
@@ -4911,15 +4907,15 @@
         <v>0</v>
       </c>
     </row>
-    <row r="83" spans="1:27" hidden="1" x14ac:dyDescent="0.5">
+    <row r="83" spans="1:27">
       <c r="A83" t="s">
         <v>2</v>
       </c>
       <c r="B83" t="s">
-        <v>99</v>
+        <v>98</v>
       </c>
       <c r="C83" t="s">
-        <v>102</v>
+        <v>101</v>
       </c>
       <c r="D83" t="s">
         <v>77</v>
@@ -4929,7 +4925,7 @@
         <v>Steam</v>
       </c>
       <c r="F83" t="s">
-        <v>142</v>
+        <v>140</v>
       </c>
       <c r="H83" s="12">
         <v>0.15</v>
@@ -4978,15 +4974,15 @@
         <v>0.13500000000000001</v>
       </c>
     </row>
-    <row r="84" spans="1:27" hidden="1" x14ac:dyDescent="0.5">
+    <row r="84" spans="1:27">
       <c r="A84" t="s">
         <v>2</v>
       </c>
       <c r="B84" t="s">
-        <v>99</v>
+        <v>98</v>
       </c>
       <c r="C84" t="s">
-        <v>102</v>
+        <v>101</v>
       </c>
       <c r="D84" t="s">
         <v>76</v>
@@ -4996,7 +4992,7 @@
         <v>Electricity</v>
       </c>
       <c r="F84" t="s">
-        <v>142</v>
+        <v>140</v>
       </c>
       <c r="H84" s="12">
         <v>0.08</v>
@@ -5045,15 +5041,15 @@
         <v>0.08</v>
       </c>
     </row>
-    <row r="85" spans="1:27" hidden="1" x14ac:dyDescent="0.5">
+    <row r="85" spans="1:27">
       <c r="A85" t="s">
         <v>2</v>
       </c>
       <c r="B85" t="s">
-        <v>99</v>
+        <v>98</v>
       </c>
       <c r="C85" t="s">
-        <v>102</v>
+        <v>101</v>
       </c>
       <c r="D85" t="s">
         <v>72</v>
@@ -5063,7 +5059,7 @@
         <v>Met coal</v>
       </c>
       <c r="F85" t="s">
-        <v>137</v>
+        <v>135</v>
       </c>
       <c r="H85" s="12"/>
       <c r="J85" s="12"/>
@@ -5082,25 +5078,25 @@
         <v>3.0281690140845072E-2</v>
       </c>
     </row>
-    <row r="86" spans="1:27" hidden="1" x14ac:dyDescent="0.5">
+    <row r="86" spans="1:27">
       <c r="A86" t="s">
         <v>2</v>
       </c>
       <c r="B86" t="s">
-        <v>99</v>
+        <v>98</v>
       </c>
       <c r="C86" t="s">
-        <v>102</v>
+        <v>101</v>
       </c>
       <c r="D86" t="s">
-        <v>94</v>
+        <v>93</v>
       </c>
       <c r="E86" t="str">
         <f t="shared" si="0"/>
         <v>BOF gas</v>
       </c>
       <c r="F86" t="s">
-        <v>142</v>
+        <v>140</v>
       </c>
       <c r="H86" s="12"/>
       <c r="J86" s="12"/>
@@ -5120,15 +5116,15 @@
       </c>
       <c r="Y86" s="15"/>
     </row>
-    <row r="87" spans="1:27" hidden="1" x14ac:dyDescent="0.5">
+    <row r="87" spans="1:27">
       <c r="A87" t="s">
         <v>2</v>
       </c>
       <c r="B87" t="s">
-        <v>99</v>
+        <v>98</v>
       </c>
       <c r="C87" t="s">
-        <v>103</v>
+        <v>102</v>
       </c>
       <c r="D87" t="s">
         <v>82</v>
@@ -5138,9 +5134,9 @@
         <v>Natural gas</v>
       </c>
       <c r="F87" t="s">
-        <v>142</v>
-      </c>
-      <c r="H87" s="12">
+        <v>140</v>
+      </c>
+      <c r="H87" s="17">
         <v>2.4E-2</v>
       </c>
       <c r="I87" s="9">
@@ -5183,15 +5179,15 @@
         <v>2.1600000000000001E-2</v>
       </c>
     </row>
-    <row r="88" spans="1:27" hidden="1" x14ac:dyDescent="0.5">
+    <row r="88" spans="1:27">
       <c r="A88" t="s">
         <v>2</v>
       </c>
       <c r="B88" t="s">
-        <v>99</v>
+        <v>98</v>
       </c>
       <c r="C88" t="s">
-        <v>103</v>
+        <v>102</v>
       </c>
       <c r="D88" t="s">
         <v>76</v>
@@ -5201,7 +5197,7 @@
         <v>Electricity</v>
       </c>
       <c r="F88" t="s">
-        <v>142</v>
+        <v>140</v>
       </c>
       <c r="H88" s="12">
         <v>0.04</v>
@@ -5250,25 +5246,25 @@
         <v>0.04</v>
       </c>
     </row>
-    <row r="89" spans="1:27" hidden="1" x14ac:dyDescent="0.5">
+    <row r="89" spans="1:27">
       <c r="A89" t="s">
         <v>2</v>
       </c>
       <c r="B89" t="s">
-        <v>99</v>
+        <v>98</v>
       </c>
       <c r="C89" t="s">
+        <v>102</v>
+      </c>
+      <c r="D89" t="s">
         <v>103</v>
-      </c>
-      <c r="D89" t="s">
-        <v>104</v>
       </c>
       <c r="E89" t="str">
         <f t="shared" si="0"/>
         <v>Other slag</v>
       </c>
       <c r="F89" t="s">
-        <v>156</v>
+        <v>154</v>
       </c>
       <c r="H89" s="12">
         <v>125</v>
@@ -5317,12 +5313,12 @@
         <v>125</v>
       </c>
     </row>
-    <row r="90" spans="1:27" hidden="1" x14ac:dyDescent="0.5">
+    <row r="90" spans="1:27">
       <c r="A90" t="s">
         <v>2</v>
       </c>
       <c r="B90" t="s">
-        <v>105</v>
+        <v>104</v>
       </c>
       <c r="C90" t="s">
         <v>71</v>
@@ -5335,7 +5331,7 @@
         <v>Natural gas</v>
       </c>
       <c r="F90" t="s">
-        <v>149</v>
+        <v>147</v>
       </c>
       <c r="H90" s="12"/>
       <c r="I90" s="12"/>
@@ -5369,12 +5365,12 @@
         <v>10.1</v>
       </c>
     </row>
-    <row r="91" spans="1:27" hidden="1" x14ac:dyDescent="0.5">
+    <row r="91" spans="1:27">
       <c r="A91" t="s">
         <v>2</v>
       </c>
       <c r="B91" t="s">
-        <v>105</v>
+        <v>104</v>
       </c>
       <c r="C91" t="s">
         <v>71</v>
@@ -5387,7 +5383,7 @@
         <v>Iron ore</v>
       </c>
       <c r="F91" t="s">
-        <v>138</v>
+        <v>136</v>
       </c>
       <c r="H91" s="12"/>
       <c r="I91" s="12"/>
@@ -5425,22 +5421,22 @@
         <v>1.4285714285714288</v>
       </c>
     </row>
-    <row r="92" spans="1:27" hidden="1" x14ac:dyDescent="0.5">
+    <row r="92" spans="1:27">
       <c r="A92" t="s">
         <v>2</v>
       </c>
       <c r="B92" t="s">
-        <v>105</v>
+        <v>104</v>
       </c>
       <c r="C92" t="s">
         <v>71</v>
       </c>
       <c r="D92" t="s">
-        <v>87</v>
+        <v>86</v>
       </c>
       <c r="E92" s="7"/>
       <c r="F92" t="s">
-        <v>138</v>
+        <v>136</v>
       </c>
       <c r="H92" s="12"/>
       <c r="I92" s="12"/>
@@ -5458,25 +5454,25 @@
         <v>0</v>
       </c>
     </row>
-    <row r="93" spans="1:27" hidden="1" x14ac:dyDescent="0.5">
+    <row r="93" spans="1:27">
       <c r="A93" t="s">
         <v>2</v>
       </c>
       <c r="B93" t="s">
-        <v>105</v>
+        <v>104</v>
       </c>
       <c r="C93" t="s">
         <v>71</v>
       </c>
       <c r="D93" t="s">
-        <v>88</v>
+        <v>87</v>
       </c>
       <c r="E93" t="str">
         <f t="shared" si="0"/>
         <v>Coke</v>
       </c>
       <c r="F93" t="s">
-        <v>138</v>
+        <v>136</v>
       </c>
       <c r="H93" s="12"/>
       <c r="I93" s="12"/>
@@ -5490,25 +5486,25 @@
         <v>0</v>
       </c>
     </row>
-    <row r="94" spans="1:27" hidden="1" x14ac:dyDescent="0.5">
+    <row r="94" spans="1:27">
       <c r="A94" t="s">
         <v>2</v>
       </c>
       <c r="B94" t="s">
-        <v>105</v>
+        <v>104</v>
       </c>
       <c r="C94" t="s">
         <v>71</v>
       </c>
       <c r="D94" t="s">
-        <v>106</v>
+        <v>105</v>
       </c>
       <c r="E94" t="str">
         <f t="shared" si="0"/>
         <v>Coal</v>
       </c>
       <c r="F94" t="s">
-        <v>138</v>
+        <v>136</v>
       </c>
       <c r="H94" s="12"/>
       <c r="I94" s="12"/>
@@ -5522,12 +5518,12 @@
         <v>0</v>
       </c>
     </row>
-    <row r="95" spans="1:27" hidden="1" x14ac:dyDescent="0.5">
+    <row r="95" spans="1:27">
       <c r="A95" t="s">
         <v>2</v>
       </c>
       <c r="B95" t="s">
-        <v>105</v>
+        <v>104</v>
       </c>
       <c r="C95" t="s">
         <v>71</v>
@@ -5540,7 +5536,7 @@
         <v>BF gas</v>
       </c>
       <c r="F95" t="s">
-        <v>138</v>
+        <v>136</v>
       </c>
       <c r="H95" s="12"/>
       <c r="I95" s="12"/>
@@ -5554,12 +5550,12 @@
         <v>0</v>
       </c>
     </row>
-    <row r="96" spans="1:27" hidden="1" x14ac:dyDescent="0.5">
+    <row r="96" spans="1:27">
       <c r="A96" t="s">
         <v>2</v>
       </c>
       <c r="B96" t="s">
-        <v>105</v>
+        <v>104</v>
       </c>
       <c r="C96" t="s">
         <v>71</v>
@@ -5572,7 +5568,7 @@
         <v>COG</v>
       </c>
       <c r="F96" t="s">
-        <v>138</v>
+        <v>136</v>
       </c>
       <c r="H96" s="12"/>
       <c r="I96" s="12"/>
@@ -5586,12 +5582,12 @@
         <v>0</v>
       </c>
     </row>
-    <row r="97" spans="1:26" hidden="1" x14ac:dyDescent="0.5">
+    <row r="97" spans="1:26">
       <c r="A97" t="s">
         <v>2</v>
       </c>
       <c r="B97" t="s">
-        <v>105</v>
+        <v>104</v>
       </c>
       <c r="C97" t="s">
         <v>71</v>
@@ -5604,7 +5600,7 @@
         <v>Natural gas</v>
       </c>
       <c r="F97" t="s">
-        <v>138</v>
+        <v>136</v>
       </c>
       <c r="H97" s="12"/>
       <c r="I97" s="12"/>
@@ -5618,25 +5614,25 @@
         <v>0</v>
       </c>
     </row>
-    <row r="98" spans="1:26" hidden="1" x14ac:dyDescent="0.5">
+    <row r="98" spans="1:26">
       <c r="A98" t="s">
         <v>2</v>
       </c>
       <c r="B98" t="s">
-        <v>105</v>
+        <v>104</v>
       </c>
       <c r="C98" t="s">
         <v>71</v>
       </c>
       <c r="D98" t="s">
-        <v>94</v>
+        <v>93</v>
       </c>
       <c r="E98" t="str">
         <f t="shared" si="0"/>
         <v>BOF gas</v>
       </c>
       <c r="F98" t="s">
-        <v>138</v>
+        <v>136</v>
       </c>
       <c r="H98" s="12"/>
       <c r="I98" s="12"/>
@@ -5650,25 +5646,25 @@
         <v>0</v>
       </c>
     </row>
-    <row r="99" spans="1:26" hidden="1" x14ac:dyDescent="0.5">
+    <row r="99" spans="1:26">
       <c r="A99" t="s">
         <v>2</v>
       </c>
       <c r="B99" t="s">
-        <v>105</v>
+        <v>104</v>
       </c>
       <c r="C99" t="s">
         <v>71</v>
       </c>
       <c r="D99" t="s">
-        <v>107</v>
+        <v>106</v>
       </c>
       <c r="E99" t="str">
         <f t="shared" si="0"/>
         <v>Biomethane</v>
       </c>
       <c r="F99" t="s">
-        <v>149</v>
+        <v>147</v>
       </c>
       <c r="H99" s="12"/>
       <c r="I99" s="12"/>
@@ -5684,15 +5680,15 @@
         <v>0</v>
       </c>
     </row>
-    <row r="100" spans="1:26" hidden="1" x14ac:dyDescent="0.5">
+    <row r="100" spans="1:26">
       <c r="A100" t="s">
         <v>2</v>
       </c>
       <c r="B100" t="s">
-        <v>105</v>
+        <v>104</v>
       </c>
       <c r="C100" t="s">
-        <v>95</v>
+        <v>94</v>
       </c>
       <c r="D100" t="s">
         <v>76</v>
@@ -5702,7 +5698,7 @@
         <v>Electricity</v>
       </c>
       <c r="F100" t="s">
-        <v>149</v>
+        <v>147</v>
       </c>
       <c r="H100" s="12"/>
       <c r="I100" s="12"/>
@@ -5741,15 +5737,15 @@
         <v>0.34033613445378152</v>
       </c>
     </row>
-    <row r="101" spans="1:26" hidden="1" x14ac:dyDescent="0.5">
+    <row r="101" spans="1:26">
       <c r="A101" t="s">
         <v>2</v>
       </c>
       <c r="B101" t="s">
-        <v>105</v>
+        <v>104</v>
       </c>
       <c r="C101" t="s">
-        <v>96</v>
+        <v>95</v>
       </c>
       <c r="D101" t="s">
         <v>77</v>
@@ -5759,7 +5755,7 @@
         <v>Steam</v>
       </c>
       <c r="F101" t="s">
-        <v>138</v>
+        <v>136</v>
       </c>
       <c r="H101" s="12"/>
       <c r="I101" s="12"/>
@@ -5769,25 +5765,25 @@
         <v>0</v>
       </c>
     </row>
-    <row r="102" spans="1:26" hidden="1" x14ac:dyDescent="0.5">
+    <row r="102" spans="1:26">
       <c r="A102" t="s">
         <v>2</v>
       </c>
       <c r="B102" t="s">
-        <v>105</v>
+        <v>104</v>
       </c>
       <c r="C102" t="s">
         <v>71</v>
       </c>
       <c r="D102" t="s">
-        <v>92</v>
+        <v>91</v>
       </c>
       <c r="E102" t="str">
         <f t="shared" si="0"/>
         <v>Hydrogen</v>
       </c>
       <c r="F102" t="s">
-        <v>149</v>
+        <v>147</v>
       </c>
       <c r="H102" s="12"/>
       <c r="I102" s="12"/>
@@ -5807,15 +5803,15 @@
         <v>7.56</v>
       </c>
     </row>
-    <row r="103" spans="1:26" hidden="1" x14ac:dyDescent="0.5">
+    <row r="103" spans="1:26">
       <c r="A103" t="s">
         <v>2</v>
       </c>
       <c r="B103" t="s">
-        <v>105</v>
+        <v>104</v>
       </c>
       <c r="C103" t="s">
-        <v>108</v>
+        <v>107</v>
       </c>
       <c r="D103" t="s">
         <v>76</v>
@@ -5825,7 +5821,7 @@
         <v>Electricity</v>
       </c>
       <c r="F103" t="s">
-        <v>149</v>
+        <v>147</v>
       </c>
       <c r="H103" s="12"/>
       <c r="I103" s="12"/>
@@ -5841,15 +5837,15 @@
         <v>1.55925</v>
       </c>
     </row>
-    <row r="104" spans="1:26" hidden="1" x14ac:dyDescent="0.5">
+    <row r="104" spans="1:26">
       <c r="A104" t="s">
         <v>2</v>
       </c>
       <c r="B104" t="s">
-        <v>105</v>
+        <v>104</v>
       </c>
       <c r="C104" t="s">
-        <v>108</v>
+        <v>107</v>
       </c>
       <c r="D104" t="s">
         <v>80</v>
@@ -5859,7 +5855,7 @@
         <v>Thermal coal</v>
       </c>
       <c r="F104" t="s">
-        <v>138</v>
+        <v>136</v>
       </c>
       <c r="H104" s="12"/>
       <c r="I104" s="12"/>
@@ -5870,15 +5866,15 @@
         <v>0</v>
       </c>
     </row>
-    <row r="105" spans="1:26" hidden="1" x14ac:dyDescent="0.5">
+    <row r="105" spans="1:26">
       <c r="A105" t="s">
         <v>2</v>
       </c>
       <c r="B105" t="s">
-        <v>105</v>
+        <v>104</v>
       </c>
       <c r="C105" t="s">
-        <v>108</v>
+        <v>107</v>
       </c>
       <c r="D105" t="s">
         <v>75</v>
@@ -5888,7 +5884,7 @@
         <v>BF gas</v>
       </c>
       <c r="F105" t="s">
-        <v>138</v>
+        <v>136</v>
       </c>
       <c r="H105" s="12"/>
       <c r="I105" s="12"/>
@@ -5899,15 +5895,15 @@
         <v>0</v>
       </c>
     </row>
-    <row r="106" spans="1:26" hidden="1" x14ac:dyDescent="0.5">
+    <row r="106" spans="1:26">
       <c r="A106" t="s">
         <v>2</v>
       </c>
       <c r="B106" t="s">
-        <v>105</v>
+        <v>104</v>
       </c>
       <c r="C106" t="s">
-        <v>108</v>
+        <v>107</v>
       </c>
       <c r="D106" t="s">
         <v>74</v>
@@ -5917,7 +5913,7 @@
         <v>COG</v>
       </c>
       <c r="F106" t="s">
-        <v>138</v>
+        <v>136</v>
       </c>
       <c r="H106" s="12"/>
       <c r="I106" s="12"/>
@@ -5928,15 +5924,15 @@
         <v>0</v>
       </c>
     </row>
-    <row r="107" spans="1:26" hidden="1" x14ac:dyDescent="0.5">
+    <row r="107" spans="1:26">
       <c r="A107" t="s">
         <v>2</v>
       </c>
       <c r="B107" t="s">
-        <v>105</v>
+        <v>104</v>
       </c>
       <c r="C107" t="s">
-        <v>108</v>
+        <v>107</v>
       </c>
       <c r="D107" t="s">
         <v>82</v>
@@ -5946,7 +5942,7 @@
         <v>Natural gas</v>
       </c>
       <c r="F107" t="s">
-        <v>149</v>
+        <v>147</v>
       </c>
       <c r="H107" s="12"/>
       <c r="I107" s="12"/>
@@ -5961,25 +5957,25 @@
         <v>0</v>
       </c>
     </row>
-    <row r="108" spans="1:26" hidden="1" x14ac:dyDescent="0.5">
+    <row r="108" spans="1:26">
       <c r="A108" t="s">
         <v>2</v>
       </c>
       <c r="B108" t="s">
-        <v>105</v>
+        <v>104</v>
       </c>
       <c r="C108" t="s">
-        <v>108</v>
+        <v>107</v>
       </c>
       <c r="D108" t="s">
-        <v>94</v>
+        <v>93</v>
       </c>
       <c r="E108" t="str">
         <f t="shared" si="24"/>
         <v>BOF gas</v>
       </c>
       <c r="F108" t="s">
-        <v>138</v>
+        <v>136</v>
       </c>
       <c r="H108" s="12"/>
       <c r="I108" s="12"/>
@@ -5990,25 +5986,25 @@
         <v>0</v>
       </c>
     </row>
-    <row r="109" spans="1:26" hidden="1" x14ac:dyDescent="0.5">
+    <row r="109" spans="1:26">
       <c r="A109" t="s">
         <v>2</v>
       </c>
       <c r="B109" t="s">
-        <v>109</v>
+        <v>108</v>
       </c>
       <c r="C109" t="s">
         <v>71</v>
       </c>
       <c r="D109" t="s">
-        <v>101</v>
+        <v>100</v>
       </c>
       <c r="E109" t="str">
         <f t="shared" si="24"/>
         <v>Scrap</v>
       </c>
       <c r="F109" t="s">
-        <v>137</v>
+        <v>135</v>
       </c>
       <c r="H109" s="12"/>
       <c r="I109" s="12"/>
@@ -6036,22 +6032,22 @@
         <v>0.3</v>
       </c>
     </row>
-    <row r="110" spans="1:26" hidden="1" x14ac:dyDescent="0.5">
+    <row r="110" spans="1:26">
       <c r="A110" t="s">
         <v>2</v>
       </c>
       <c r="B110" t="s">
-        <v>109</v>
+        <v>108</v>
       </c>
       <c r="C110" t="s">
         <v>71</v>
       </c>
       <c r="D110" t="s">
-        <v>110</v>
+        <v>109</v>
       </c>
       <c r="E110" s="7"/>
       <c r="F110" t="s">
-        <v>137</v>
+        <v>135</v>
       </c>
       <c r="H110" s="12"/>
       <c r="I110" s="12"/>
@@ -6078,12 +6074,12 @@
         <v>1.1363636363636365</v>
       </c>
     </row>
-    <row r="111" spans="1:26" hidden="1" x14ac:dyDescent="0.5">
+    <row r="111" spans="1:26">
       <c r="A111" t="s">
         <v>2</v>
       </c>
       <c r="B111" t="s">
-        <v>109</v>
+        <v>108</v>
       </c>
       <c r="C111" t="s">
         <v>71</v>
@@ -6096,7 +6092,7 @@
         <v>Met coal</v>
       </c>
       <c r="F111" t="s">
-        <v>137</v>
+        <v>135</v>
       </c>
       <c r="H111" s="12"/>
       <c r="I111" s="12"/>
@@ -6116,22 +6112,22 @@
         <v>2.119718309859155E-2</v>
       </c>
     </row>
-    <row r="112" spans="1:26" hidden="1" x14ac:dyDescent="0.5">
+    <row r="112" spans="1:26">
       <c r="A112" t="s">
         <v>2</v>
       </c>
       <c r="B112" t="s">
-        <v>109</v>
+        <v>108</v>
       </c>
       <c r="C112" t="s">
         <v>71</v>
       </c>
       <c r="D112" s="7" t="s">
-        <v>170</v>
+        <v>168</v>
       </c>
       <c r="E112" s="7"/>
       <c r="F112" t="s">
-        <v>137</v>
+        <v>135</v>
       </c>
       <c r="H112" s="12"/>
       <c r="I112" s="12"/>
@@ -6149,15 +6145,15 @@
         <v>0.67899999999999994</v>
       </c>
     </row>
-    <row r="113" spans="1:27" hidden="1" x14ac:dyDescent="0.5">
+    <row r="113" spans="1:27">
       <c r="A113" t="s">
         <v>2</v>
       </c>
       <c r="B113" t="s">
-        <v>109</v>
+        <v>108</v>
       </c>
       <c r="C113" t="s">
-        <v>111</v>
+        <v>110</v>
       </c>
       <c r="D113" t="s">
         <v>82</v>
@@ -6167,7 +6163,7 @@
         <v>Natural gas</v>
       </c>
       <c r="F113" t="s">
-        <v>142</v>
+        <v>140</v>
       </c>
       <c r="H113" s="12"/>
       <c r="I113" s="12"/>
@@ -6185,12 +6181,12 @@
         <v>0.05</v>
       </c>
     </row>
-    <row r="114" spans="1:27" hidden="1" x14ac:dyDescent="0.5">
+    <row r="114" spans="1:27">
       <c r="A114" t="s">
         <v>2</v>
       </c>
       <c r="B114" t="s">
-        <v>109</v>
+        <v>108</v>
       </c>
       <c r="C114" t="s">
         <v>20</v>
@@ -6203,7 +6199,7 @@
         <v>Met coal</v>
       </c>
       <c r="F114" t="s">
-        <v>137</v>
+        <v>135</v>
       </c>
       <c r="H114" s="12"/>
       <c r="I114" s="12"/>
@@ -6215,12 +6211,12 @@
         <v>3.0281690140845072E-2</v>
       </c>
     </row>
-    <row r="115" spans="1:27" hidden="1" x14ac:dyDescent="0.5">
+    <row r="115" spans="1:27">
       <c r="A115" t="s">
         <v>2</v>
       </c>
       <c r="B115" t="s">
-        <v>109</v>
+        <v>108</v>
       </c>
       <c r="C115" t="s">
         <v>20</v>
@@ -6233,7 +6229,7 @@
         <v>COG</v>
       </c>
       <c r="F115" t="s">
-        <v>142</v>
+        <v>140</v>
       </c>
       <c r="H115" s="12"/>
       <c r="I115" s="12"/>
@@ -6247,12 +6243,12 @@
         <v>0</v>
       </c>
     </row>
-    <row r="116" spans="1:27" hidden="1" x14ac:dyDescent="0.5">
+    <row r="116" spans="1:27">
       <c r="A116" t="s">
         <v>2</v>
       </c>
       <c r="B116" t="s">
-        <v>109</v>
+        <v>108</v>
       </c>
       <c r="C116" t="s">
         <v>20</v>
@@ -6265,7 +6261,7 @@
         <v>BF gas</v>
       </c>
       <c r="F116" t="s">
-        <v>142</v>
+        <v>140</v>
       </c>
       <c r="H116" s="12"/>
       <c r="I116" s="12"/>
@@ -6279,12 +6275,12 @@
         <v>0</v>
       </c>
     </row>
-    <row r="117" spans="1:27" hidden="1" x14ac:dyDescent="0.5">
+    <row r="117" spans="1:27">
       <c r="A117" t="s">
         <v>2</v>
       </c>
       <c r="B117" t="s">
-        <v>109</v>
+        <v>108</v>
       </c>
       <c r="C117" t="s">
         <v>20</v>
@@ -6297,7 +6293,7 @@
         <v>Steam</v>
       </c>
       <c r="F117" t="s">
-        <v>142</v>
+        <v>140</v>
       </c>
       <c r="H117" s="12"/>
       <c r="I117" s="12"/>
@@ -6332,12 +6328,12 @@
         <v>0.3</v>
       </c>
     </row>
-    <row r="118" spans="1:27" hidden="1" x14ac:dyDescent="0.5">
+    <row r="118" spans="1:27">
       <c r="A118" t="s">
         <v>2</v>
       </c>
       <c r="B118" t="s">
-        <v>109</v>
+        <v>108</v>
       </c>
       <c r="C118" t="s">
         <v>20</v>
@@ -6350,7 +6346,7 @@
         <v>Electricity</v>
       </c>
       <c r="F118" t="s">
-        <v>142</v>
+        <v>140</v>
       </c>
       <c r="H118" s="12"/>
       <c r="I118" s="12"/>
@@ -6389,25 +6385,25 @@
         <v>1.2707999999999999</v>
       </c>
     </row>
-    <row r="119" spans="1:27" hidden="1" x14ac:dyDescent="0.5">
+    <row r="119" spans="1:27">
       <c r="A119" t="s">
         <v>2</v>
       </c>
       <c r="B119" t="s">
-        <v>109</v>
+        <v>108</v>
       </c>
       <c r="C119" t="s">
-        <v>103</v>
+        <v>102</v>
       </c>
       <c r="D119" t="s">
-        <v>107</v>
+        <v>106</v>
       </c>
       <c r="E119" t="str">
         <f t="shared" si="24"/>
         <v>Biomethane</v>
       </c>
       <c r="F119" t="s">
-        <v>142</v>
+        <v>140</v>
       </c>
       <c r="H119" s="12"/>
       <c r="I119" s="12"/>
@@ -6424,15 +6420,15 @@
       </c>
       <c r="Q119" s="17"/>
     </row>
-    <row r="120" spans="1:27" hidden="1" x14ac:dyDescent="0.5">
+    <row r="120" spans="1:27">
       <c r="A120" t="s">
         <v>2</v>
       </c>
       <c r="B120" t="s">
-        <v>109</v>
+        <v>108</v>
       </c>
       <c r="C120" t="s">
-        <v>103</v>
+        <v>102</v>
       </c>
       <c r="D120" t="s">
         <v>82</v>
@@ -6442,7 +6438,7 @@
         <v>Natural gas</v>
       </c>
       <c r="F120" t="s">
-        <v>142</v>
+        <v>140</v>
       </c>
       <c r="H120" s="12"/>
       <c r="I120" s="12"/>
@@ -6470,15 +6466,15 @@
         <v>1.4039999999999999</v>
       </c>
     </row>
-    <row r="121" spans="1:27" hidden="1" x14ac:dyDescent="0.5">
+    <row r="121" spans="1:27">
       <c r="A121" t="s">
         <v>2</v>
       </c>
       <c r="B121" t="s">
-        <v>109</v>
+        <v>108</v>
       </c>
       <c r="C121" t="s">
-        <v>103</v>
+        <v>102</v>
       </c>
       <c r="D121" t="s">
         <v>76</v>
@@ -6488,7 +6484,7 @@
         <v>Electricity</v>
       </c>
       <c r="F121" t="s">
-        <v>142</v>
+        <v>140</v>
       </c>
       <c r="H121" s="12"/>
       <c r="I121" s="12"/>
@@ -6527,15 +6523,15 @@
         <v>1.1232</v>
       </c>
     </row>
-    <row r="122" spans="1:27" hidden="1" x14ac:dyDescent="0.5">
+    <row r="122" spans="1:27">
       <c r="A122" t="s">
         <v>2</v>
       </c>
       <c r="B122" t="s">
-        <v>109</v>
+        <v>108</v>
       </c>
       <c r="C122" t="s">
-        <v>103</v>
+        <v>102</v>
       </c>
       <c r="D122" t="s">
         <v>76</v>
@@ -6545,7 +6541,7 @@
         <v>Electricity</v>
       </c>
       <c r="F122" t="s">
-        <v>142</v>
+        <v>140</v>
       </c>
       <c r="H122" s="12"/>
       <c r="I122" s="12"/>
@@ -6557,15 +6553,15 @@
         <v>0.35460000000000003</v>
       </c>
     </row>
-    <row r="123" spans="1:27" hidden="1" x14ac:dyDescent="0.5">
+    <row r="123" spans="1:27">
       <c r="A123" t="s">
         <v>2</v>
       </c>
       <c r="B123" t="s">
-        <v>109</v>
+        <v>108</v>
       </c>
       <c r="C123" t="s">
-        <v>103</v>
+        <v>102</v>
       </c>
       <c r="D123" t="s">
         <v>76</v>
@@ -6575,7 +6571,7 @@
         <v>Electricity</v>
       </c>
       <c r="F123" t="s">
-        <v>142</v>
+        <v>140</v>
       </c>
       <c r="H123" s="12"/>
       <c r="I123" s="12"/>
@@ -6592,25 +6588,25 @@
         <v>0.35460000000000003</v>
       </c>
     </row>
-    <row r="124" spans="1:27" hidden="1" x14ac:dyDescent="0.5">
+    <row r="124" spans="1:27">
       <c r="A124" t="s">
         <v>2</v>
       </c>
       <c r="B124" t="s">
-        <v>109</v>
+        <v>108</v>
       </c>
       <c r="C124" t="s">
+        <v>102</v>
+      </c>
+      <c r="D124" t="s">
         <v>103</v>
-      </c>
-      <c r="D124" t="s">
-        <v>104</v>
       </c>
       <c r="E124" t="str">
         <f t="shared" si="24"/>
         <v>Other slag</v>
       </c>
       <c r="F124" t="s">
-        <v>156</v>
+        <v>154</v>
       </c>
       <c r="H124" s="12"/>
       <c r="I124" s="12"/>
@@ -6639,25 +6635,25 @@
         <v>180</v>
       </c>
     </row>
-    <row r="125" spans="1:27" hidden="1" x14ac:dyDescent="0.5">
+    <row r="125" spans="1:27">
       <c r="A125" t="s">
         <v>2</v>
       </c>
       <c r="B125" t="s">
-        <v>109</v>
+        <v>108</v>
       </c>
       <c r="C125" t="s">
-        <v>103</v>
+        <v>102</v>
       </c>
       <c r="D125" t="s">
-        <v>112</v>
+        <v>111</v>
       </c>
       <c r="E125" t="str">
         <f t="shared" si="24"/>
         <v>Process emissions</v>
       </c>
       <c r="F125" t="s">
-        <v>165</v>
+        <v>163</v>
       </c>
       <c r="H125" s="12"/>
       <c r="I125" s="12"/>
@@ -6692,22 +6688,22 @@
         <v>0.08</v>
       </c>
     </row>
-    <row r="126" spans="1:27" hidden="1" x14ac:dyDescent="0.5">
+    <row r="126" spans="1:27">
       <c r="A126" t="s">
         <v>2</v>
       </c>
       <c r="B126" t="s">
-        <v>113</v>
+        <v>112</v>
       </c>
       <c r="C126" t="s">
         <v>71</v>
       </c>
       <c r="D126" t="s">
-        <v>114</v>
+        <v>113</v>
       </c>
       <c r="E126" s="7"/>
       <c r="F126" t="s">
-        <v>155</v>
+        <v>153</v>
       </c>
       <c r="H126" s="12">
         <v>25.7</v>
@@ -6731,22 +6727,22 @@
         <v>25.7</v>
       </c>
     </row>
-    <row r="127" spans="1:27" hidden="1" x14ac:dyDescent="0.5">
+    <row r="127" spans="1:27">
       <c r="A127" t="s">
         <v>2</v>
       </c>
       <c r="B127" t="s">
-        <v>113</v>
+        <v>112</v>
       </c>
       <c r="C127" t="s">
         <v>71</v>
       </c>
       <c r="D127" t="s">
-        <v>115</v>
+        <v>114</v>
       </c>
       <c r="E127" s="7"/>
       <c r="F127" t="s">
-        <v>156</v>
+        <v>154</v>
       </c>
       <c r="H127" s="12">
         <v>67</v>
@@ -6787,12 +6783,12 @@
         <v>67</v>
       </c>
     </row>
-    <row r="128" spans="1:27" hidden="1" x14ac:dyDescent="0.5">
+    <row r="128" spans="1:27">
       <c r="A128" t="s">
         <v>2</v>
       </c>
       <c r="B128" t="s">
-        <v>116</v>
+        <v>115</v>
       </c>
       <c r="C128" t="s">
         <v>71</v>
@@ -6805,7 +6801,7 @@
         <v>COG</v>
       </c>
       <c r="F128" t="s">
-        <v>153</v>
+        <v>151</v>
       </c>
       <c r="H128" s="12">
         <f>1/$H$18*(H14+10%)</f>
@@ -6836,12 +6832,12 @@
         <v>0.8</v>
       </c>
     </row>
-    <row r="129" spans="1:27" hidden="1" x14ac:dyDescent="0.5">
+    <row r="129" spans="1:27">
       <c r="A129" t="s">
         <v>2</v>
       </c>
       <c r="B129" t="s">
-        <v>116</v>
+        <v>115</v>
       </c>
       <c r="C129" t="s">
         <v>71</v>
@@ -6854,7 +6850,7 @@
         <v>BF gas</v>
       </c>
       <c r="F129" t="s">
-        <v>153</v>
+        <v>151</v>
       </c>
       <c r="H129" s="12">
         <f>1/$H$18*(H15-10%)</f>
@@ -6885,25 +6881,25 @@
         <v>1.2</v>
       </c>
     </row>
-    <row r="130" spans="1:27" hidden="1" x14ac:dyDescent="0.5">
+    <row r="130" spans="1:27">
       <c r="A130" t="s">
         <v>2</v>
       </c>
       <c r="B130" t="s">
-        <v>116</v>
+        <v>115</v>
       </c>
       <c r="C130" t="s">
         <v>71</v>
       </c>
       <c r="D130" t="s">
-        <v>94</v>
+        <v>93</v>
       </c>
       <c r="E130" t="str">
         <f t="shared" si="24"/>
         <v>BOF gas</v>
       </c>
       <c r="F130" t="s">
-        <v>153</v>
+        <v>151</v>
       </c>
       <c r="H130" s="12"/>
       <c r="J130" s="12"/>
@@ -6916,12 +6912,12 @@
         <v>2</v>
       </c>
     </row>
-    <row r="131" spans="1:27" hidden="1" x14ac:dyDescent="0.5">
+    <row r="131" spans="1:27">
       <c r="A131" t="s">
         <v>2</v>
       </c>
       <c r="B131" t="s">
-        <v>116</v>
+        <v>115</v>
       </c>
       <c r="C131" t="s">
         <v>71</v>
@@ -6934,7 +6930,7 @@
         <v>Thermal coal</v>
       </c>
       <c r="F131" t="s">
-        <v>154</v>
+        <v>152</v>
       </c>
       <c r="H131" s="12">
         <f>1/$H$19</f>
@@ -6965,21 +6961,21 @@
         <v>1.0000000000000001E-5</v>
       </c>
     </row>
-    <row r="132" spans="1:27" hidden="1" x14ac:dyDescent="0.5">
+    <row r="132" spans="1:27">
       <c r="A132" t="s">
         <v>2</v>
       </c>
       <c r="B132" t="s">
+        <v>116</v>
+      </c>
+      <c r="D132" t="s">
         <v>117</v>
       </c>
-      <c r="D132" t="s">
-        <v>118</v>
-      </c>
       <c r="E132" t="s">
-        <v>121</v>
+        <v>120</v>
       </c>
       <c r="F132" t="s">
-        <v>160</v>
+        <v>158</v>
       </c>
       <c r="H132" s="12"/>
       <c r="L132" s="12">
@@ -6998,15 +6994,15 @@
         <v>1</v>
       </c>
     </row>
-    <row r="133" spans="1:27" hidden="1" x14ac:dyDescent="0.5">
+    <row r="133" spans="1:27">
       <c r="A133" t="s">
         <v>2</v>
       </c>
       <c r="B133" t="s">
-        <v>117</v>
+        <v>116</v>
       </c>
       <c r="C133" t="s">
-        <v>119</v>
+        <v>118</v>
       </c>
       <c r="D133" t="s">
         <v>82</v>
@@ -7016,7 +7012,7 @@
         <v>Natural gas</v>
       </c>
       <c r="F133" t="s">
-        <v>161</v>
+        <v>159</v>
       </c>
       <c r="H133" s="12"/>
       <c r="L133" s="12">
@@ -7032,15 +7028,15 @@
         <v>3.6</v>
       </c>
     </row>
-    <row r="134" spans="1:27" hidden="1" x14ac:dyDescent="0.5">
+    <row r="134" spans="1:27">
       <c r="A134" t="s">
         <v>2</v>
       </c>
       <c r="B134" t="s">
-        <v>117</v>
+        <v>116</v>
       </c>
       <c r="C134" t="s">
-        <v>120</v>
+        <v>119</v>
       </c>
       <c r="D134" t="s">
         <v>76</v>
@@ -7050,7 +7046,7 @@
         <v>Electricity</v>
       </c>
       <c r="F134" t="s">
-        <v>161</v>
+        <v>159</v>
       </c>
       <c r="H134" s="12"/>
       <c r="L134" s="12">
@@ -7073,22 +7069,22 @@
         <v>0.36</v>
       </c>
     </row>
-    <row r="135" spans="1:27" hidden="1" x14ac:dyDescent="0.5">
+    <row r="135" spans="1:27">
       <c r="A135" t="s">
         <v>2</v>
       </c>
       <c r="B135" t="s">
-        <v>117</v>
+        <v>116</v>
       </c>
       <c r="D135" t="s">
-        <v>121</v>
+        <v>120</v>
       </c>
       <c r="E135" t="str">
         <f t="shared" si="24"/>
         <v>Captured CO2</v>
       </c>
       <c r="F135" t="s">
-        <v>160</v>
+        <v>158</v>
       </c>
       <c r="H135" s="12"/>
       <c r="L135" s="9">
@@ -7112,7 +7108,7 @@
         <v>0.9</v>
       </c>
     </row>
-    <row r="136" spans="1:27" hidden="1" x14ac:dyDescent="0.5">
+    <row r="136" spans="1:27">
       <c r="A136" t="s">
         <v>29</v>
       </c>
@@ -7122,43 +7118,43 @@
       <c r="C136" t="s">
         <v>73</v>
       </c>
-      <c r="D136" s="6" t="s">
-        <v>122</v>
+      <c r="D136" t="s">
+        <v>174</v>
       </c>
       <c r="F136" s="6" t="s">
-        <v>166</v>
+        <v>164</v>
       </c>
       <c r="G136" s="5">
         <v>0.47265002739006901</v>
       </c>
     </row>
-    <row r="137" spans="1:27" hidden="1" x14ac:dyDescent="0.5">
+    <row r="137" spans="1:27">
       <c r="A137" t="s">
         <v>2</v>
       </c>
       <c r="B137" t="s">
-        <v>169</v>
+        <v>167</v>
       </c>
       <c r="C137" t="s">
         <v>71</v>
       </c>
       <c r="D137" t="s">
-        <v>86</v>
+        <v>85</v>
       </c>
       <c r="E137" s="7"/>
       <c r="F137" t="s">
-        <v>136</v>
+        <v>134</v>
       </c>
       <c r="R137" s="9">
         <v>0</v>
       </c>
     </row>
-    <row r="138" spans="1:27" hidden="1" x14ac:dyDescent="0.5">
+    <row r="138" spans="1:27">
       <c r="A138" t="s">
         <v>2</v>
       </c>
       <c r="B138" t="s">
-        <v>169</v>
+        <v>167</v>
       </c>
       <c r="C138" t="s">
         <v>71</v>
@@ -7171,7 +7167,7 @@
         <v>Iron ore</v>
       </c>
       <c r="F138" t="s">
-        <v>136</v>
+        <v>134</v>
       </c>
       <c r="R138" s="9">
         <v>1.42</v>
@@ -7180,84 +7176,84 @@
         <v>1.42</v>
       </c>
     </row>
-    <row r="139" spans="1:27" hidden="1" x14ac:dyDescent="0.5">
+    <row r="139" spans="1:27">
       <c r="A139" t="s">
         <v>2</v>
       </c>
       <c r="B139" t="s">
-        <v>169</v>
+        <v>167</v>
       </c>
       <c r="C139" t="s">
         <v>71</v>
       </c>
       <c r="D139" t="s">
-        <v>87</v>
+        <v>86</v>
       </c>
       <c r="E139" s="7"/>
       <c r="F139" t="s">
-        <v>136</v>
+        <v>134</v>
       </c>
       <c r="R139" s="9">
         <v>0</v>
       </c>
     </row>
-    <row r="140" spans="1:27" hidden="1" x14ac:dyDescent="0.5">
+    <row r="140" spans="1:27">
       <c r="A140" t="s">
         <v>2</v>
       </c>
       <c r="B140" t="s">
-        <v>169</v>
+        <v>167</v>
       </c>
       <c r="C140" t="s">
         <v>71</v>
       </c>
       <c r="D140" t="s">
-        <v>88</v>
+        <v>87</v>
       </c>
       <c r="E140" t="str">
         <f t="shared" si="24"/>
         <v>Coke</v>
       </c>
       <c r="F140" t="s">
-        <v>136</v>
+        <v>134</v>
       </c>
       <c r="R140" s="9">
         <v>0</v>
       </c>
     </row>
-    <row r="141" spans="1:27" hidden="1" x14ac:dyDescent="0.5">
+    <row r="141" spans="1:27">
       <c r="A141" t="s">
         <v>2</v>
       </c>
       <c r="B141" t="s">
-        <v>169</v>
+        <v>167</v>
       </c>
       <c r="C141" t="s">
         <v>71</v>
       </c>
       <c r="D141" t="s">
-        <v>89</v>
+        <v>88</v>
       </c>
       <c r="E141" t="str">
         <f t="shared" si="24"/>
         <v>DRI</v>
       </c>
       <c r="F141" t="s">
-        <v>136</v>
+        <v>134</v>
       </c>
       <c r="R141" s="9">
         <v>0</v>
       </c>
     </row>
-    <row r="142" spans="1:27" hidden="1" x14ac:dyDescent="0.5">
+    <row r="142" spans="1:27">
       <c r="A142" t="s">
         <v>2</v>
       </c>
       <c r="B142" t="s">
-        <v>169</v>
+        <v>167</v>
       </c>
       <c r="C142" t="s">
-        <v>91</v>
+        <v>90</v>
       </c>
       <c r="D142" t="s">
         <v>80</v>
@@ -7267,7 +7263,7 @@
         <v>Thermal coal</v>
       </c>
       <c r="F142" t="s">
-        <v>148</v>
+        <v>146</v>
       </c>
       <c r="R142" s="9">
         <v>12.7</v>
@@ -7276,15 +7272,15 @@
         <v>12.7</v>
       </c>
     </row>
-    <row r="143" spans="1:27" hidden="1" x14ac:dyDescent="0.5">
+    <row r="143" spans="1:27">
       <c r="A143" t="s">
         <v>2</v>
       </c>
       <c r="B143" t="s">
-        <v>169</v>
+        <v>167</v>
       </c>
       <c r="C143" t="s">
-        <v>93</v>
+        <v>92</v>
       </c>
       <c r="D143" t="s">
         <v>75</v>
@@ -7294,21 +7290,21 @@
         <v>BF gas</v>
       </c>
       <c r="F143" t="s">
-        <v>148</v>
+        <v>146</v>
       </c>
       <c r="R143" s="9">
         <v>0</v>
       </c>
     </row>
-    <row r="144" spans="1:27" hidden="1" x14ac:dyDescent="0.5">
+    <row r="144" spans="1:27">
       <c r="A144" t="s">
         <v>2</v>
       </c>
       <c r="B144" t="s">
-        <v>169</v>
+        <v>167</v>
       </c>
       <c r="C144" t="s">
-        <v>93</v>
+        <v>92</v>
       </c>
       <c r="D144" t="s">
         <v>74</v>
@@ -7318,21 +7314,21 @@
         <v>COG</v>
       </c>
       <c r="F144" t="s">
-        <v>148</v>
+        <v>146</v>
       </c>
       <c r="R144" s="9">
         <v>0</v>
       </c>
     </row>
-    <row r="145" spans="1:26" hidden="1" x14ac:dyDescent="0.5">
+    <row r="145" spans="1:26">
       <c r="A145" t="s">
         <v>2</v>
       </c>
       <c r="B145" t="s">
-        <v>169</v>
+        <v>167</v>
       </c>
       <c r="C145" t="s">
-        <v>93</v>
+        <v>92</v>
       </c>
       <c r="D145" t="s">
         <v>82</v>
@@ -7342,7 +7338,7 @@
         <v>Natural gas</v>
       </c>
       <c r="F145" t="s">
-        <v>148</v>
+        <v>146</v>
       </c>
       <c r="R145" s="12">
         <f>0.95-R80-R87</f>
@@ -7352,39 +7348,39 @@
         <v>0.89</v>
       </c>
     </row>
-    <row r="146" spans="1:26" hidden="1" x14ac:dyDescent="0.5">
+    <row r="146" spans="1:26">
       <c r="A146" t="s">
         <v>2</v>
       </c>
       <c r="B146" t="s">
-        <v>169</v>
+        <v>167</v>
       </c>
       <c r="C146" t="s">
+        <v>92</v>
+      </c>
+      <c r="D146" t="s">
         <v>93</v>
-      </c>
-      <c r="D146" t="s">
-        <v>94</v>
       </c>
       <c r="E146" t="str">
         <f t="shared" si="24"/>
         <v>BOF gas</v>
       </c>
       <c r="F146" t="s">
-        <v>148</v>
+        <v>146</v>
       </c>
       <c r="R146" s="9">
         <v>0</v>
       </c>
     </row>
-    <row r="147" spans="1:26" hidden="1" x14ac:dyDescent="0.5">
+    <row r="147" spans="1:26">
       <c r="A147" t="s">
         <v>2</v>
       </c>
       <c r="B147" t="s">
-        <v>169</v>
+        <v>167</v>
       </c>
       <c r="C147" t="s">
-        <v>95</v>
+        <v>94</v>
       </c>
       <c r="D147" t="s">
         <v>76</v>
@@ -7394,7 +7390,7 @@
         <v>Electricity</v>
       </c>
       <c r="F147" t="s">
-        <v>148</v>
+        <v>146</v>
       </c>
       <c r="R147" s="12">
         <f>0.95-R84-R88</f>
@@ -7404,15 +7400,15 @@
         <v>0.83</v>
       </c>
     </row>
-    <row r="148" spans="1:26" hidden="1" x14ac:dyDescent="0.5">
+    <row r="148" spans="1:26">
       <c r="A148" t="s">
         <v>2</v>
       </c>
       <c r="B148" t="s">
-        <v>169</v>
+        <v>167</v>
       </c>
       <c r="C148" t="s">
-        <v>96</v>
+        <v>95</v>
       </c>
       <c r="D148" t="s">
         <v>77</v>
@@ -7422,7 +7418,7 @@
         <v>Steam</v>
       </c>
       <c r="F148" t="s">
-        <v>148</v>
+        <v>146</v>
       </c>
       <c r="R148" s="9">
         <v>0</v>
@@ -7431,12 +7427,12 @@
         <v>0</v>
       </c>
     </row>
-    <row r="149" spans="1:26" hidden="1" x14ac:dyDescent="0.5">
+    <row r="149" spans="1:26">
       <c r="A149" t="s">
         <v>2</v>
       </c>
       <c r="B149" t="s">
-        <v>123</v>
+        <v>121</v>
       </c>
       <c r="C149" t="s">
         <v>71</v>
@@ -7449,7 +7445,7 @@
         <v>Iron ore</v>
       </c>
       <c r="F149" t="s">
-        <v>139</v>
+        <v>137</v>
       </c>
       <c r="U149" s="9">
         <v>1.44</v>
@@ -7458,15 +7454,15 @@
         <v>1.51</v>
       </c>
     </row>
-    <row r="150" spans="1:26" hidden="1" x14ac:dyDescent="0.5">
+    <row r="150" spans="1:26">
       <c r="A150" t="s">
         <v>2</v>
       </c>
       <c r="B150" t="s">
-        <v>123</v>
+        <v>121</v>
       </c>
       <c r="C150" t="s">
-        <v>95</v>
+        <v>94</v>
       </c>
       <c r="D150" t="s">
         <v>76</v>
@@ -7476,22 +7472,22 @@
         <v>Electricity</v>
       </c>
       <c r="F150" t="s">
-        <v>150</v>
+        <v>148</v>
       </c>
       <c r="U150" s="9">
         <f>(90*3.6/1000)/0.952</f>
         <v>0.34033613445378152</v>
       </c>
     </row>
-    <row r="151" spans="1:26" hidden="1" x14ac:dyDescent="0.5">
+    <row r="151" spans="1:26">
       <c r="A151" t="s">
         <v>2</v>
       </c>
       <c r="B151" t="s">
-        <v>123</v>
+        <v>121</v>
       </c>
       <c r="C151" t="s">
-        <v>124</v>
+        <v>122</v>
       </c>
       <c r="D151" t="s">
         <v>76</v>
@@ -7501,7 +7497,7 @@
         <v>Electricity</v>
       </c>
       <c r="F151" t="s">
-        <v>150</v>
+        <v>148</v>
       </c>
       <c r="U151" s="9">
         <v>13.33</v>
@@ -7510,33 +7506,33 @@
         <v>11.96</v>
       </c>
     </row>
-    <row r="152" spans="1:26" hidden="1" x14ac:dyDescent="0.5">
+    <row r="152" spans="1:26">
       <c r="A152" t="s">
         <v>2</v>
       </c>
       <c r="B152" t="s">
-        <v>125</v>
+        <v>123</v>
       </c>
       <c r="D152" t="s">
-        <v>126</v>
+        <v>124</v>
       </c>
       <c r="E152" t="s">
-        <v>130</v>
+        <v>128</v>
       </c>
       <c r="F152" t="s">
-        <v>162</v>
+        <v>160</v>
       </c>
       <c r="V152" s="9">
         <f>0.52*44/12</f>
         <v>1.906666666666667</v>
       </c>
     </row>
-    <row r="153" spans="1:26" hidden="1" x14ac:dyDescent="0.5">
+    <row r="153" spans="1:26">
       <c r="A153" t="s">
         <v>2</v>
       </c>
       <c r="B153" t="s">
-        <v>125</v>
+        <v>123</v>
       </c>
       <c r="D153" t="s">
         <v>76</v>
@@ -7546,43 +7542,43 @@
         <v>Electricity</v>
       </c>
       <c r="F153" t="s">
-        <v>151</v>
+        <v>149</v>
       </c>
       <c r="V153" s="9">
         <f>2*3.6</f>
         <v>7.2</v>
       </c>
     </row>
-    <row r="154" spans="1:26" hidden="1" x14ac:dyDescent="0.5">
+    <row r="154" spans="1:26">
       <c r="A154" t="s">
         <v>2</v>
       </c>
       <c r="B154" t="s">
-        <v>127</v>
+        <v>125</v>
       </c>
       <c r="D154" t="s">
-        <v>118</v>
+        <v>117</v>
       </c>
       <c r="E154" t="s">
-        <v>121</v>
+        <v>120</v>
       </c>
       <c r="F154" t="s">
-        <v>160</v>
+        <v>158</v>
       </c>
       <c r="V154" s="12">
         <f>L132</f>
         <v>1</v>
       </c>
     </row>
-    <row r="155" spans="1:26" hidden="1" x14ac:dyDescent="0.5">
+    <row r="155" spans="1:26">
       <c r="A155" t="s">
         <v>2</v>
       </c>
       <c r="B155" t="s">
-        <v>127</v>
+        <v>125</v>
       </c>
       <c r="C155" t="s">
-        <v>119</v>
+        <v>118</v>
       </c>
       <c r="D155" t="s">
         <v>76</v>
@@ -7592,22 +7588,22 @@
         <v>Electricity</v>
       </c>
       <c r="F155" t="s">
-        <v>161</v>
+        <v>159</v>
       </c>
       <c r="V155" s="12">
         <f t="shared" ref="V155:V157" si="29">L133</f>
         <v>3.6</v>
       </c>
     </row>
-    <row r="156" spans="1:26" hidden="1" x14ac:dyDescent="0.5">
+    <row r="156" spans="1:26">
       <c r="A156" t="s">
         <v>2</v>
       </c>
       <c r="B156" t="s">
-        <v>127</v>
+        <v>125</v>
       </c>
       <c r="C156" t="s">
-        <v>120</v>
+        <v>119</v>
       </c>
       <c r="D156" t="s">
         <v>76</v>
@@ -7617,51 +7613,51 @@
         <v>Electricity</v>
       </c>
       <c r="F156" t="s">
-        <v>161</v>
+        <v>159</v>
       </c>
       <c r="V156" s="12">
         <f t="shared" si="29"/>
         <v>0.36</v>
       </c>
     </row>
-    <row r="157" spans="1:26" hidden="1" x14ac:dyDescent="0.5">
+    <row r="157" spans="1:26">
       <c r="A157" t="s">
         <v>2</v>
       </c>
       <c r="B157" t="s">
-        <v>127</v>
+        <v>125</v>
       </c>
       <c r="D157" t="s">
-        <v>121</v>
+        <v>120</v>
       </c>
       <c r="E157" t="str">
         <f t="shared" si="24"/>
         <v>Captured CO2</v>
       </c>
       <c r="F157" t="s">
-        <v>160</v>
+        <v>158</v>
       </c>
       <c r="V157" s="12">
         <f t="shared" si="29"/>
         <v>0.9</v>
       </c>
     </row>
-    <row r="158" spans="1:26" hidden="1" x14ac:dyDescent="0.5">
+    <row r="158" spans="1:26">
       <c r="A158" t="s">
         <v>2</v>
       </c>
       <c r="B158" t="s">
-        <v>128</v>
+        <v>126</v>
       </c>
       <c r="C158" t="s">
         <v>71</v>
       </c>
       <c r="D158" t="s">
-        <v>110</v>
+        <v>109</v>
       </c>
       <c r="E158" s="7"/>
       <c r="F158" t="s">
-        <v>136</v>
+        <v>134</v>
       </c>
       <c r="W158" s="9">
         <v>1</v>
@@ -7674,15 +7670,15 @@
         <v>1</v>
       </c>
     </row>
-    <row r="159" spans="1:26" hidden="1" x14ac:dyDescent="0.5">
+    <row r="159" spans="1:26">
       <c r="A159" t="s">
         <v>2</v>
       </c>
       <c r="B159" t="s">
-        <v>128</v>
+        <v>126</v>
       </c>
       <c r="C159" t="s">
-        <v>129</v>
+        <v>127</v>
       </c>
       <c r="D159" t="s">
         <v>82</v>
@@ -7692,7 +7688,7 @@
         <v>Natural gas</v>
       </c>
       <c r="F159" t="s">
-        <v>148</v>
+        <v>146</v>
       </c>
       <c r="W159" s="9">
         <f>((1538-$W$36)*W39/1000+$W$41+($W$37-1538)*$W$40/1000)/$W$38-W160</f>
@@ -7703,25 +7699,25 @@
         <v>1.3350380259623991</v>
       </c>
     </row>
-    <row r="160" spans="1:26" hidden="1" x14ac:dyDescent="0.5">
+    <row r="160" spans="1:26">
       <c r="A160" t="s">
         <v>2</v>
       </c>
       <c r="B160" t="s">
-        <v>128</v>
+        <v>126</v>
       </c>
       <c r="C160" t="s">
-        <v>129</v>
+        <v>127</v>
       </c>
       <c r="D160" t="s">
-        <v>94</v>
+        <v>93</v>
       </c>
       <c r="E160" t="str">
         <f t="shared" si="24"/>
         <v>BOF gas</v>
       </c>
       <c r="F160" t="s">
-        <v>148</v>
+        <v>146</v>
       </c>
       <c r="W160" s="9">
         <v>0.2</v>
@@ -7731,15 +7727,15 @@
         <v>0.2</v>
       </c>
     </row>
-    <row r="161" spans="1:25" hidden="1" x14ac:dyDescent="0.5">
+    <row r="161" spans="1:25">
       <c r="A161" t="s">
         <v>2</v>
       </c>
       <c r="B161" t="s">
-        <v>128</v>
+        <v>126</v>
       </c>
       <c r="C161" t="s">
-        <v>129</v>
+        <v>127</v>
       </c>
       <c r="D161" t="s">
         <v>76</v>
@@ -7749,7 +7745,7 @@
         <v>Electricity</v>
       </c>
       <c r="F161" t="s">
-        <v>148</v>
+        <v>146</v>
       </c>
       <c r="Y161" s="9">
         <f>((1538-$Y$36)*Y39/1000+$Y$41+($Y$37-1538)*$Y$40/1000)/$Y$38</f>
@@ -7757,13 +7753,7 @@
       </c>
     </row>
   </sheetData>
-  <autoFilter ref="A2:AB161" xr:uid="{F5E4BE5B-48FB-4F9E-83ED-5B539B3F5C30}">
-    <filterColumn colId="3">
-      <filters>
-        <filter val="Share of electricity purchased in total demand"/>
-      </filters>
-    </filterColumn>
-  </autoFilter>
+  <autoFilter ref="A2:AB161" xr:uid="{F5E4BE5B-48FB-4F9E-83ED-5B539B3F5C30}"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
   <legacyDrawing r:id="rId2"/>
@@ -7771,25 +7761,6 @@
 </file>
 
 <file path=customXml/item1.xml><?xml version="1.0" encoding="utf-8"?>
-<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
-  <documentManagement>
-    <SharedWithUsers xmlns="f6f44a7d-d6f5-4042-8792-19cb5f90fb06">
-      <UserInfo>
-        <DisplayName>Andrew Isabirye</DisplayName>
-        <AccountId>30706</AccountId>
-        <AccountType/>
-      </UserInfo>
-      <UserInfo>
-        <DisplayName>Hannah Maral</DisplayName>
-        <AccountId>22065</AccountId>
-        <AccountType/>
-      </UserInfo>
-    </SharedWithUsers>
-  </documentManagement>
-</p:properties>
-</file>
-
-<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
 <?mso-contentType ?>
 <FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
   <Display>DocumentLibraryForm</Display>
@@ -7798,9 +7769,9 @@
 </FormTemplates>
 </file>
 
-<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
-<ct:contentTypeSchema xmlns:ct="http://schemas.microsoft.com/office/2006/metadata/contentType" xmlns:ma="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes" ct:_="" ma:_="" ma:contentTypeName="Document" ma:contentTypeID="0x0101001B4ECEDC51D0484091AFD4177D66ED73" ma:contentTypeVersion="" ma:contentTypeDescription="Create a new document." ma:contentTypeScope="" ma:versionID="679fe9fe38f968c92fa3ecf94914311c">
-  <xsd:schema xmlns:xsd="http://www.w3.org/2001/XMLSchema" xmlns:xs="http://www.w3.org/2001/XMLSchema" xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:ns2="b44fa922-a688-4301-8945-67f7597c9c55" xmlns:ns3="f6f44a7d-d6f5-4042-8792-19cb5f90fb06" targetNamespace="http://schemas.microsoft.com/office/2006/metadata/properties" ma:root="true" ma:fieldsID="e752f064d4542b785f81007626879ee0" ns2:_="" ns3:_="">
+<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
+<ct:contentTypeSchema xmlns:ct="http://schemas.microsoft.com/office/2006/metadata/contentType" xmlns:ma="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes" ct:_="" ma:_="" ma:contentTypeName="Document" ma:contentTypeID="0x0101001B4ECEDC51D0484091AFD4177D66ED73" ma:contentTypeVersion="" ma:contentTypeDescription="Create a new document." ma:contentTypeScope="" ma:versionID="319a675c9647c7594acaff66597be50a">
+  <xsd:schema xmlns:xsd="http://www.w3.org/2001/XMLSchema" xmlns:xs="http://www.w3.org/2001/XMLSchema" xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:ns2="b44fa922-a688-4301-8945-67f7597c9c55" xmlns:ns3="f6f44a7d-d6f5-4042-8792-19cb5f90fb06" targetNamespace="http://schemas.microsoft.com/office/2006/metadata/properties" ma:root="true" ma:fieldsID="88dc2720d39439db86350823647c6b2d" ns2:_="" ns3:_="">
     <xsd:import namespace="b44fa922-a688-4301-8945-67f7597c9c55"/>
     <xsd:import namespace="f6f44a7d-d6f5-4042-8792-19cb5f90fb06"/>
     <xsd:element name="properties">
@@ -7815,6 +7786,10 @@
                 <xsd:element ref="ns3:SharedWithDetails" minOccurs="0"/>
                 <xsd:element ref="ns2:MediaServiceAutoKeyPoints" minOccurs="0"/>
                 <xsd:element ref="ns2:MediaServiceKeyPoints" minOccurs="0"/>
+                <xsd:element ref="ns2:MediaServiceAutoTags" minOccurs="0"/>
+                <xsd:element ref="ns2:MediaServiceOCR" minOccurs="0"/>
+                <xsd:element ref="ns2:MediaServiceGenerationTime" minOccurs="0"/>
+                <xsd:element ref="ns2:MediaServiceEventHashCode" minOccurs="0"/>
               </xsd:all>
             </xsd:complexType>
           </xsd:element>
@@ -7845,6 +7820,28 @@
         <xsd:restriction base="dms:Note">
           <xsd:maxLength value="255"/>
         </xsd:restriction>
+      </xsd:simpleType>
+    </xsd:element>
+    <xsd:element name="MediaServiceAutoTags" ma:index="14" nillable="true" ma:displayName="Tags" ma:internalName="MediaServiceAutoTags" ma:readOnly="true">
+      <xsd:simpleType>
+        <xsd:restriction base="dms:Text"/>
+      </xsd:simpleType>
+    </xsd:element>
+    <xsd:element name="MediaServiceOCR" ma:index="15" nillable="true" ma:displayName="Extracted Text" ma:internalName="MediaServiceOCR" ma:readOnly="true">
+      <xsd:simpleType>
+        <xsd:restriction base="dms:Note">
+          <xsd:maxLength value="255"/>
+        </xsd:restriction>
+      </xsd:simpleType>
+    </xsd:element>
+    <xsd:element name="MediaServiceGenerationTime" ma:index="16" nillable="true" ma:displayName="MediaServiceGenerationTime" ma:hidden="true" ma:internalName="MediaServiceGenerationTime" ma:readOnly="true">
+      <xsd:simpleType>
+        <xsd:restriction base="dms:Text"/>
+      </xsd:simpleType>
+    </xsd:element>
+    <xsd:element name="MediaServiceEventHashCode" ma:index="17" nillable="true" ma:displayName="MediaServiceEventHashCode" ma:hidden="true" ma:internalName="MediaServiceEventHashCode" ma:readOnly="true">
+      <xsd:simpleType>
+        <xsd:restriction base="dms:Text"/>
       </xsd:simpleType>
     </xsd:element>
   </xsd:schema>
@@ -7977,24 +7974,26 @@
 </ct:contentTypeSchema>
 </file>
 
-<file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{25282EF4-73CF-4347-829C-ED59BCC7A63D}">
-  <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://purl.org/dc/elements/1.1/"/>
-    <ds:schemaRef ds:uri="f6f44a7d-d6f5-4042-8792-19cb5f90fb06"/>
-    <ds:schemaRef ds:uri="http://purl.org/dc/terms/"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/documentManagement/types"/>
-    <ds:schemaRef ds:uri="http://schemas.openxmlformats.org/package/2006/metadata/core-properties"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
-    <ds:schemaRef ds:uri="b44fa922-a688-4301-8945-67f7597c9c55"/>
-    <ds:schemaRef ds:uri="http://www.w3.org/XML/1998/namespace"/>
-    <ds:schemaRef ds:uri="http://purl.org/dc/dcmitype/"/>
-  </ds:schemaRefs>
-</ds:datastoreItem>
+<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
+<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
+  <documentManagement>
+    <SharedWithUsers xmlns="f6f44a7d-d6f5-4042-8792-19cb5f90fb06">
+      <UserInfo>
+        <DisplayName>Andrew Isabirye</DisplayName>
+        <AccountId>30706</AccountId>
+        <AccountType/>
+      </UserInfo>
+      <UserInfo>
+        <DisplayName>Hannah Maral</DisplayName>
+        <AccountId>22065</AccountId>
+        <AccountType/>
+      </UserInfo>
+    </SharedWithUsers>
+  </documentManagement>
+</p:properties>
 </file>
 
-<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
 <ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{991F2D94-C2BE-428C-8D22-7BDD52D7C413}">
   <ds:schemaRefs>
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
@@ -8002,8 +8001,8 @@
 </ds:datastoreItem>
 </file>
 
-<file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{9C4F83C3-6035-48AA-AD0A-B7D40025FD47}">
+<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{DB25B099-1FAC-465C-8173-479800A6E319}">
   <ds:schemaRefs>
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/contentType"/>
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes"/>
@@ -8019,4 +8018,21 @@
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/internal/obd"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
+</file>
+
+<file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{25282EF4-73CF-4347-829C-ED59BCC7A63D}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://purl.org/dc/elements/1.1/"/>
+    <ds:schemaRef ds:uri="f6f44a7d-d6f5-4042-8792-19cb5f90fb06"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/terms/"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/documentManagement/types"/>
+    <ds:schemaRef ds:uri="http://schemas.openxmlformats.org/package/2006/metadata/core-properties"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+    <ds:schemaRef ds:uri="b44fa922-a688-4301-8945-67f7597c9c55"/>
+    <ds:schemaRef ds:uri="http://www.w3.org/XML/1998/namespace"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/dcmitype/"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
 </file>
</xml_diff>

<commit_message>
business case updates - rebased to match excel
</commit_message>
<xml_diff>
--- a/mppsteel/data/import_data/Business Cases One Table.xlsx
+++ b/mppsteel/data/import_data/Business Cases One Table.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://systemiq.sharepoint.com/Projects/MPP0006/Shared Documents/6_ Working documents/03 Steel python model/Data Sources/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="1655" documentId="8_{E5ECF8DE-F7F7-4DAE-A1FD-DC27A0AAFB42}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{D797A1E5-9EE8-4A0C-916F-535336CC4417}"/>
+  <xr:revisionPtr revIDLastSave="1764" documentId="8_{E5ECF8DE-F7F7-4DAE-A1FD-DC27A0AAFB42}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{2B517807-451F-4A32-99F5-A20D63BA1CD0}"/>
   <bookViews>
-    <workbookView xWindow="28680" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{0B6EB920-BFAC-40B8-A9D9-6AEA75F19191}"/>
+    <workbookView xWindow="-93" yWindow="-93" windowWidth="25786" windowHeight="13373" xr2:uid="{0B6EB920-BFAC-40B8-A9D9-6AEA75F19191}"/>
   </bookViews>
   <sheets>
     <sheet name="Data" sheetId="1" r:id="rId1"/>
@@ -91,7 +91,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="821" uniqueCount="175">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="871" uniqueCount="195">
   <si>
     <t>Steel Business Cases</t>
   </si>
@@ -616,6 +616,66 @@
   </si>
   <si>
     <t>Power consumption for oxygen separation in ASU</t>
+  </si>
+  <si>
+    <t>0…</t>
+  </si>
+  <si>
+    <t>…......</t>
+  </si>
+  <si>
+    <t>.</t>
+  </si>
+  <si>
+    <t>0.0.0.0.0.0.0.0.0.0.0.0.0.0.0.0.0000.</t>
+  </si>
+  <si>
+    <t>…..................</t>
+  </si>
+  <si>
+    <t>..</t>
+  </si>
+  <si>
+    <t>…...................</t>
+  </si>
+  <si>
+    <t>…....................</t>
+  </si>
+  <si>
+    <t>….................................................................................................................................</t>
+  </si>
+  <si>
+    <t>….............................................</t>
+  </si>
+  <si>
+    <t>…</t>
+  </si>
+  <si>
+    <t>…...........</t>
+  </si>
+  <si>
+    <t>…..........................</t>
+  </si>
+  <si>
+    <t>0…............................................................00000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000..</t>
+  </si>
+  <si>
+    <t>…...</t>
+  </si>
+  <si>
+    <t>….</t>
+  </si>
+  <si>
+    <t>….............................................................................................................</t>
+  </si>
+  <si>
+    <t>….................................</t>
+  </si>
+  <si>
+    <t>00000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000.............</t>
+  </si>
+  <si>
+    <t>…..</t>
   </si>
 </sst>
 </file>
@@ -625,7 +685,7 @@
   <numFmts count="1">
     <numFmt numFmtId="164" formatCode="0.000"/>
   </numFmts>
-  <fonts count="9">
+  <fonts count="9" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -1119,46 +1179,47 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{F5E4BE5B-48FB-4F9E-83ED-5B539B3F5C30}">
-  <dimension ref="A1:AB161"/>
+  <sheetPr filterMode="1"/>
+  <dimension ref="A1:AB2598"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
-      <pane xSplit="6" ySplit="2" topLeftCell="G111" activePane="bottomRight" state="frozen"/>
+      <pane xSplit="6" ySplit="2" topLeftCell="P10" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="G1" sqref="G1"/>
       <selection pane="bottomLeft" activeCell="A4" sqref="A4"/>
-      <selection pane="bottomRight" activeCell="D136" sqref="D136"/>
+      <selection pane="bottomRight" activeCell="Q165" sqref="Q165"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.5"/>
+  <sheetFormatPr defaultRowHeight="14.35" x14ac:dyDescent="0.5"/>
   <cols>
     <col min="1" max="1" width="25" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="30.54296875" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="30.54296875" customWidth="1"/>
-    <col min="4" max="4" width="39.54296875" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="30.52734375" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="30.52734375" customWidth="1"/>
+    <col min="4" max="4" width="39.52734375" bestFit="1" customWidth="1"/>
     <col min="5" max="5" width="26" customWidth="1"/>
-    <col min="6" max="6" width="18.6328125" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="7.54296875" customWidth="1"/>
-    <col min="8" max="8" width="9.1796875" style="9" customWidth="1"/>
-    <col min="9" max="9" width="14.1796875" style="9" bestFit="1" customWidth="1"/>
-    <col min="10" max="10" width="11.1796875" style="9" bestFit="1" customWidth="1"/>
-    <col min="11" max="11" width="14.1796875" style="9" bestFit="1" customWidth="1"/>
-    <col min="12" max="12" width="11.1796875" style="9" bestFit="1" customWidth="1"/>
-    <col min="13" max="16" width="9.1796875" style="9" customWidth="1"/>
-    <col min="17" max="17" width="9.7265625" style="9" bestFit="1" customWidth="1"/>
-    <col min="18" max="19" width="11.1796875" style="9" bestFit="1" customWidth="1"/>
-    <col min="20" max="20" width="9.1796875" style="9" customWidth="1"/>
-    <col min="21" max="21" width="14.1796875" style="9" bestFit="1" customWidth="1"/>
-    <col min="22" max="22" width="11.1796875" style="9" bestFit="1" customWidth="1"/>
-    <col min="23" max="23" width="14.1796875" style="9" bestFit="1" customWidth="1"/>
-    <col min="24" max="26" width="9.1796875" style="9" customWidth="1"/>
-    <col min="27" max="27" width="11.1796875" style="9" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="18.64453125" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="7.52734375" customWidth="1"/>
+    <col min="8" max="8" width="9.17578125" style="9" customWidth="1"/>
+    <col min="9" max="9" width="14.17578125" style="9" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="11.17578125" style="9" bestFit="1" customWidth="1"/>
+    <col min="11" max="11" width="14.17578125" style="9" bestFit="1" customWidth="1"/>
+    <col min="12" max="12" width="11.17578125" style="9" bestFit="1" customWidth="1"/>
+    <col min="13" max="16" width="9.17578125" style="9" customWidth="1"/>
+    <col min="17" max="17" width="9.703125" style="9" bestFit="1" customWidth="1"/>
+    <col min="18" max="19" width="11.17578125" style="9" bestFit="1" customWidth="1"/>
+    <col min="20" max="20" width="9.17578125" style="9" customWidth="1"/>
+    <col min="21" max="21" width="14.17578125" style="9" bestFit="1" customWidth="1"/>
+    <col min="22" max="22" width="11.17578125" style="9" bestFit="1" customWidth="1"/>
+    <col min="23" max="23" width="14.17578125" style="9" bestFit="1" customWidth="1"/>
+    <col min="24" max="26" width="9.17578125" style="9" customWidth="1"/>
+    <col min="27" max="27" width="11.17578125" style="9" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:28" ht="35.25" customHeight="1">
+    <row r="1" spans="1:28" ht="35.25" customHeight="1" x14ac:dyDescent="0.95">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
     </row>
-    <row r="2" spans="1:28" ht="149.5">
+    <row r="2" spans="1:28" ht="146" x14ac:dyDescent="0.5">
       <c r="A2" s="2" t="s">
         <v>1</v>
       </c>
@@ -1244,7 +1305,7 @@
         <v>28</v>
       </c>
     </row>
-    <row r="3" spans="1:28">
+    <row r="3" spans="1:28" hidden="1" x14ac:dyDescent="0.5">
       <c r="A3" t="s">
         <v>29</v>
       </c>
@@ -1290,7 +1351,7 @@
         <v>0.3</v>
       </c>
     </row>
-    <row r="4" spans="1:28">
+    <row r="4" spans="1:28" hidden="1" x14ac:dyDescent="0.5">
       <c r="A4" t="s">
         <v>29</v>
       </c>
@@ -1325,7 +1386,7 @@
         <v>270</v>
       </c>
     </row>
-    <row r="5" spans="1:28">
+    <row r="5" spans="1:28" hidden="1" x14ac:dyDescent="0.5">
       <c r="A5" t="s">
         <v>29</v>
       </c>
@@ -1347,7 +1408,7 @@
         <v>27.5</v>
       </c>
     </row>
-    <row r="6" spans="1:28">
+    <row r="6" spans="1:28" hidden="1" x14ac:dyDescent="0.5">
       <c r="A6" t="s">
         <v>29</v>
       </c>
@@ -1370,7 +1431,7 @@
         <v>0.22916666666666666</v>
       </c>
     </row>
-    <row r="7" spans="1:28">
+    <row r="7" spans="1:28" hidden="1" x14ac:dyDescent="0.5">
       <c r="A7" t="s">
         <v>29</v>
       </c>
@@ -1393,7 +1454,7 @@
         <v>0.9</v>
       </c>
     </row>
-    <row r="8" spans="1:28">
+    <row r="8" spans="1:28" hidden="1" x14ac:dyDescent="0.5">
       <c r="A8" t="s">
         <v>29</v>
       </c>
@@ -1431,7 +1492,7 @@
         <v>0.9</v>
       </c>
     </row>
-    <row r="9" spans="1:28">
+    <row r="9" spans="1:28" hidden="1" x14ac:dyDescent="0.5">
       <c r="A9" t="s">
         <v>29</v>
       </c>
@@ -1471,7 +1532,7 @@
         <v>28.4</v>
       </c>
     </row>
-    <row r="10" spans="1:28">
+    <row r="10" spans="1:28" x14ac:dyDescent="0.5">
       <c r="A10" t="s">
         <v>29</v>
       </c>
@@ -1500,7 +1561,7 @@
       </c>
       <c r="L10" s="11">
         <f>V10</f>
-        <v>0.01</v>
+        <v>1</v>
       </c>
       <c r="R10" s="11">
         <v>0.94</v>
@@ -1509,13 +1570,13 @@
         <v>0.96</v>
       </c>
       <c r="V10" s="19">
-        <v>0.01</v>
+        <v>1</v>
       </c>
       <c r="AA10" s="15">
         <v>0.4</v>
       </c>
     </row>
-    <row r="11" spans="1:28">
+    <row r="11" spans="1:28" hidden="1" x14ac:dyDescent="0.5">
       <c r="A11" t="s">
         <v>29</v>
       </c>
@@ -1547,7 +1608,7 @@
         <v>0.9</v>
       </c>
     </row>
-    <row r="12" spans="1:28">
+    <row r="12" spans="1:28" hidden="1" x14ac:dyDescent="0.5">
       <c r="A12" t="s">
         <v>29</v>
       </c>
@@ -1590,7 +1651,7 @@
         <v>50</v>
       </c>
     </row>
-    <row r="13" spans="1:28">
+    <row r="13" spans="1:28" hidden="1" x14ac:dyDescent="0.5">
       <c r="A13" t="s">
         <v>29</v>
       </c>
@@ -1610,7 +1671,7 @@
         <v>0.15</v>
       </c>
     </row>
-    <row r="14" spans="1:28">
+    <row r="14" spans="1:28" hidden="1" x14ac:dyDescent="0.5">
       <c r="A14" t="s">
         <v>29</v>
       </c>
@@ -1653,7 +1714,7 @@
         <v>0.4</v>
       </c>
     </row>
-    <row r="15" spans="1:28">
+    <row r="15" spans="1:28" hidden="1" x14ac:dyDescent="0.5">
       <c r="A15" t="s">
         <v>29</v>
       </c>
@@ -1696,7 +1757,7 @@
         <v>0.6</v>
       </c>
     </row>
-    <row r="16" spans="1:28">
+    <row r="16" spans="1:28" hidden="1" x14ac:dyDescent="0.5">
       <c r="A16" t="s">
         <v>29</v>
       </c>
@@ -1736,7 +1797,7 @@
         <v>26</v>
       </c>
     </row>
-    <row r="17" spans="1:27">
+    <row r="17" spans="1:27" hidden="1" x14ac:dyDescent="0.5">
       <c r="A17" t="s">
         <v>29</v>
       </c>
@@ -1799,7 +1860,7 @@
         <v>0.08</v>
       </c>
     </row>
-    <row r="18" spans="1:27">
+    <row r="18" spans="1:27" hidden="1" x14ac:dyDescent="0.5">
       <c r="A18" t="s">
         <v>29</v>
       </c>
@@ -1847,7 +1908,7 @@
         <v>0.5</v>
       </c>
     </row>
-    <row r="19" spans="1:27">
+    <row r="19" spans="1:27" hidden="1" x14ac:dyDescent="0.5">
       <c r="A19" t="s">
         <v>29</v>
       </c>
@@ -1891,7 +1952,7 @@
         <v>100000</v>
       </c>
     </row>
-    <row r="20" spans="1:27">
+    <row r="20" spans="1:27" hidden="1" x14ac:dyDescent="0.5">
       <c r="A20" t="s">
         <v>29</v>
       </c>
@@ -1928,7 +1989,7 @@
         <v>0.3</v>
       </c>
     </row>
-    <row r="21" spans="1:27">
+    <row r="21" spans="1:27" hidden="1" x14ac:dyDescent="0.5">
       <c r="A21" t="s">
         <v>29</v>
       </c>
@@ -1964,7 +2025,7 @@
         <v>1.23</v>
       </c>
     </row>
-    <row r="22" spans="1:27">
+    <row r="22" spans="1:27" x14ac:dyDescent="0.5">
       <c r="A22" t="s">
         <v>29</v>
       </c>
@@ -1988,7 +2049,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="23" spans="1:27">
+    <row r="23" spans="1:27" hidden="1" x14ac:dyDescent="0.5">
       <c r="A23" t="s">
         <v>29</v>
       </c>
@@ -2027,7 +2088,7 @@
         <v>2.69</v>
       </c>
     </row>
-    <row r="24" spans="1:27">
+    <row r="24" spans="1:27" hidden="1" x14ac:dyDescent="0.5">
       <c r="A24" t="s">
         <v>29</v>
       </c>
@@ -2051,7 +2112,7 @@
         <v>0.88</v>
       </c>
     </row>
-    <row r="25" spans="1:27">
+    <row r="25" spans="1:27" hidden="1" x14ac:dyDescent="0.5">
       <c r="A25" t="s">
         <v>29</v>
       </c>
@@ -2104,7 +2165,7 @@
         <v>0.86206896551724133</v>
       </c>
     </row>
-    <row r="26" spans="1:27">
+    <row r="26" spans="1:27" hidden="1" x14ac:dyDescent="0.5">
       <c r="A26" t="s">
         <v>29</v>
       </c>
@@ -2133,7 +2194,7 @@
         <v>63</v>
       </c>
     </row>
-    <row r="27" spans="1:27">
+    <row r="27" spans="1:27" hidden="1" x14ac:dyDescent="0.5">
       <c r="A27" t="s">
         <v>29</v>
       </c>
@@ -2161,7 +2222,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="28" spans="1:27">
+    <row r="28" spans="1:27" hidden="1" x14ac:dyDescent="0.5">
       <c r="A28" t="s">
         <v>29</v>
       </c>
@@ -2189,7 +2250,7 @@
         <v>0.97</v>
       </c>
     </row>
-    <row r="29" spans="1:27">
+    <row r="29" spans="1:27" hidden="1" x14ac:dyDescent="0.5">
       <c r="A29" t="s">
         <v>29</v>
       </c>
@@ -2215,7 +2276,7 @@
         <v>12.15</v>
       </c>
     </row>
-    <row r="30" spans="1:27">
+    <row r="30" spans="1:27" hidden="1" x14ac:dyDescent="0.5">
       <c r="A30" t="s">
         <v>29</v>
       </c>
@@ -2237,7 +2298,7 @@
       <c r="L30" s="12"/>
       <c r="M30" s="11"/>
     </row>
-    <row r="31" spans="1:27">
+    <row r="31" spans="1:27" hidden="1" x14ac:dyDescent="0.5">
       <c r="A31" t="s">
         <v>29</v>
       </c>
@@ -2265,7 +2326,7 @@
         <v>120</v>
       </c>
     </row>
-    <row r="32" spans="1:27">
+    <row r="32" spans="1:27" hidden="1" x14ac:dyDescent="0.5">
       <c r="A32" t="s">
         <v>29</v>
       </c>
@@ -2293,7 +2354,7 @@
         <v>47.1</v>
       </c>
     </row>
-    <row r="33" spans="1:27">
+    <row r="33" spans="1:27" hidden="1" x14ac:dyDescent="0.5">
       <c r="A33" t="s">
         <v>29</v>
       </c>
@@ -2318,7 +2379,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="34" spans="1:27">
+    <row r="34" spans="1:27" hidden="1" x14ac:dyDescent="0.5">
       <c r="A34" t="s">
         <v>29</v>
       </c>
@@ -2343,7 +2404,7 @@
         <v>0.97</v>
       </c>
     </row>
-    <row r="35" spans="1:27">
+    <row r="35" spans="1:27" hidden="1" x14ac:dyDescent="0.5">
       <c r="A35" t="s">
         <v>29</v>
       </c>
@@ -2369,7 +2430,7 @@
       </c>
       <c r="Q35" s="12"/>
     </row>
-    <row r="36" spans="1:27">
+    <row r="36" spans="1:27" hidden="1" x14ac:dyDescent="0.5">
       <c r="A36" t="s">
         <v>29</v>
       </c>
@@ -2402,7 +2463,7 @@
         <v>700</v>
       </c>
     </row>
-    <row r="37" spans="1:27">
+    <row r="37" spans="1:27" hidden="1" x14ac:dyDescent="0.5">
       <c r="A37" t="s">
         <v>29</v>
       </c>
@@ -2435,7 +2496,7 @@
         <v>2000</v>
       </c>
     </row>
-    <row r="38" spans="1:27">
+    <row r="38" spans="1:27" hidden="1" x14ac:dyDescent="0.5">
       <c r="A38" t="s">
         <v>29</v>
       </c>
@@ -2467,7 +2528,7 @@
         <v>0.97</v>
       </c>
     </row>
-    <row r="39" spans="1:27">
+    <row r="39" spans="1:27" hidden="1" x14ac:dyDescent="0.5">
       <c r="A39" t="s">
         <v>29</v>
       </c>
@@ -2501,7 +2562,7 @@
         <v>0.45</v>
       </c>
     </row>
-    <row r="40" spans="1:27">
+    <row r="40" spans="1:27" hidden="1" x14ac:dyDescent="0.5">
       <c r="A40" t="s">
         <v>29</v>
       </c>
@@ -2535,7 +2596,7 @@
         <v>0.82</v>
       </c>
     </row>
-    <row r="41" spans="1:27">
+    <row r="41" spans="1:27" hidden="1" x14ac:dyDescent="0.5">
       <c r="A41" t="s">
         <v>29</v>
       </c>
@@ -2570,7 +2631,7 @@
         <v>0.24709042076991944</v>
       </c>
     </row>
-    <row r="42" spans="1:27" ht="11.5" customHeight="1">
+    <row r="42" spans="1:27" ht="11.5" hidden="1" customHeight="1" x14ac:dyDescent="0.5">
       <c r="A42" t="s">
         <v>2</v>
       </c>
@@ -2636,7 +2697,7 @@
         <v>1.2849999999999999</v>
       </c>
     </row>
-    <row r="43" spans="1:27">
+    <row r="43" spans="1:27" hidden="1" x14ac:dyDescent="0.5">
       <c r="A43" t="s">
         <v>2</v>
       </c>
@@ -2703,7 +2764,7 @@
         <v>2.9699999999999998</v>
       </c>
     </row>
-    <row r="44" spans="1:27">
+    <row r="44" spans="1:27" hidden="1" x14ac:dyDescent="0.5">
       <c r="A44" t="s">
         <v>2</v>
       </c>
@@ -2766,7 +2827,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="45" spans="1:27">
+    <row r="45" spans="1:27" hidden="1" x14ac:dyDescent="0.5">
       <c r="A45" t="s">
         <v>2</v>
       </c>
@@ -2832,7 +2893,7 @@
         <v>0.125</v>
       </c>
     </row>
-    <row r="46" spans="1:27">
+    <row r="46" spans="1:27" hidden="1" x14ac:dyDescent="0.5">
       <c r="A46" t="s">
         <v>2</v>
       </c>
@@ -2898,7 +2959,7 @@
         <v>0.378</v>
       </c>
     </row>
-    <row r="47" spans="1:27">
+    <row r="47" spans="1:27" hidden="1" x14ac:dyDescent="0.5">
       <c r="A47" t="s">
         <v>2</v>
       </c>
@@ -2965,7 +3026,7 @@
         <v>0.87532258064516144</v>
       </c>
     </row>
-    <row r="48" spans="1:27">
+    <row r="48" spans="1:27" hidden="1" x14ac:dyDescent="0.5">
       <c r="A48" t="s">
         <v>2</v>
       </c>
@@ -3032,7 +3093,7 @@
         <v>1.1493</v>
       </c>
     </row>
-    <row r="49" spans="1:27">
+    <row r="49" spans="1:27" hidden="1" x14ac:dyDescent="0.5">
       <c r="A49" t="s">
         <v>2</v>
       </c>
@@ -3099,7 +3160,7 @@
         <v>0.60299999999999998</v>
       </c>
     </row>
-    <row r="50" spans="1:27">
+    <row r="50" spans="1:27" hidden="1" x14ac:dyDescent="0.5">
       <c r="A50" t="s">
         <v>2</v>
       </c>
@@ -3162,7 +3223,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="51" spans="1:27">
+    <row r="51" spans="1:27" hidden="1" x14ac:dyDescent="0.5">
       <c r="A51" t="s">
         <v>2</v>
       </c>
@@ -3229,7 +3290,7 @@
         <v>0.04</v>
       </c>
     </row>
-    <row r="52" spans="1:27">
+    <row r="52" spans="1:27" hidden="1" x14ac:dyDescent="0.5">
       <c r="A52" t="s">
         <v>2</v>
       </c>
@@ -3313,7 +3374,7 @@
         <v>1.0266129032258065</v>
       </c>
     </row>
-    <row r="53" spans="1:27">
+    <row r="53" spans="1:27" hidden="1" x14ac:dyDescent="0.5">
       <c r="A53" t="s">
         <v>2</v>
       </c>
@@ -3394,7 +3455,7 @@
         <v>0.27900000000000003</v>
       </c>
     </row>
-    <row r="54" spans="1:27">
+    <row r="54" spans="1:27" hidden="1" x14ac:dyDescent="0.5">
       <c r="A54" t="s">
         <v>2</v>
       </c>
@@ -3471,7 +3532,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="55" spans="1:27">
+    <row r="55" spans="1:27" hidden="1" x14ac:dyDescent="0.5">
       <c r="A55" t="s">
         <v>2</v>
       </c>
@@ -3553,7 +3614,7 @@
         <v>9.0000000000000011E-3</v>
       </c>
     </row>
-    <row r="56" spans="1:27">
+    <row r="56" spans="1:27" hidden="1" x14ac:dyDescent="0.5">
       <c r="A56" t="s">
         <v>2</v>
       </c>
@@ -3629,7 +3690,7 @@
         <v>0.30600000000000005</v>
       </c>
     </row>
-    <row r="57" spans="1:27">
+    <row r="57" spans="1:27" hidden="1" x14ac:dyDescent="0.5">
       <c r="A57" t="s">
         <v>2</v>
       </c>
@@ -3682,7 +3743,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="58" spans="1:27">
+    <row r="58" spans="1:27" hidden="1" x14ac:dyDescent="0.5">
       <c r="A58" t="s">
         <v>2</v>
       </c>
@@ -3765,7 +3826,7 @@
         <v>7.5999999999999998E-2</v>
       </c>
     </row>
-    <row r="59" spans="1:27">
+    <row r="59" spans="1:27" hidden="1" x14ac:dyDescent="0.5">
       <c r="A59" t="s">
         <v>2</v>
       </c>
@@ -3804,7 +3865,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="60" spans="1:27">
+    <row r="60" spans="1:27" hidden="1" x14ac:dyDescent="0.5">
       <c r="A60" t="s">
         <v>2</v>
       </c>
@@ -3852,7 +3913,7 @@
         <v>0.99199999999999999</v>
       </c>
     </row>
-    <row r="61" spans="1:27">
+    <row r="61" spans="1:27" hidden="1" x14ac:dyDescent="0.5">
       <c r="A61" t="s">
         <v>2</v>
       </c>
@@ -3903,7 +3964,7 @@
         <v>0.15</v>
       </c>
     </row>
-    <row r="62" spans="1:27">
+    <row r="62" spans="1:27" hidden="1" x14ac:dyDescent="0.5">
       <c r="A62" t="s">
         <v>2</v>
       </c>
@@ -3951,7 +4012,7 @@
         <v>0.435</v>
       </c>
     </row>
-    <row r="63" spans="1:27">
+    <row r="63" spans="1:27" hidden="1" x14ac:dyDescent="0.5">
       <c r="A63" t="s">
         <v>2</v>
       </c>
@@ -4003,7 +4064,7 @@
         <v>0.21509999999999999</v>
       </c>
     </row>
-    <row r="64" spans="1:27">
+    <row r="64" spans="1:27" hidden="1" x14ac:dyDescent="0.5">
       <c r="A64" t="s">
         <v>2</v>
       </c>
@@ -4045,7 +4106,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="65" spans="1:27">
+    <row r="65" spans="1:27" hidden="1" x14ac:dyDescent="0.5">
       <c r="A65" t="s">
         <v>2</v>
       </c>
@@ -4076,7 +4137,7 @@
         <v>0.67876000000000003</v>
       </c>
     </row>
-    <row r="66" spans="1:27">
+    <row r="66" spans="1:27" hidden="1" x14ac:dyDescent="0.5">
       <c r="A66" t="s">
         <v>2</v>
       </c>
@@ -4111,7 +4172,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="67" spans="1:27">
+    <row r="67" spans="1:27" hidden="1" x14ac:dyDescent="0.5">
       <c r="A67" t="s">
         <v>2</v>
       </c>
@@ -4152,7 +4213,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="68" spans="1:27">
+    <row r="68" spans="1:27" hidden="1" x14ac:dyDescent="0.5">
       <c r="A68" t="s">
         <v>2</v>
       </c>
@@ -4188,7 +4249,7 @@
         <v>270</v>
       </c>
     </row>
-    <row r="69" spans="1:27">
+    <row r="69" spans="1:27" hidden="1" x14ac:dyDescent="0.5">
       <c r="A69" t="s">
         <v>2</v>
       </c>
@@ -4216,7 +4277,7 @@
         <v>230</v>
       </c>
     </row>
-    <row r="70" spans="1:27">
+    <row r="70" spans="1:27" hidden="1" x14ac:dyDescent="0.5">
       <c r="A70" t="s">
         <v>2</v>
       </c>
@@ -4263,7 +4324,7 @@
         <v>3.2261039999999999</v>
       </c>
     </row>
-    <row r="71" spans="1:27">
+    <row r="71" spans="1:27" hidden="1" x14ac:dyDescent="0.5">
       <c r="A71" t="s">
         <v>2</v>
       </c>
@@ -4313,7 +4374,7 @@
         <v>0.8</v>
       </c>
     </row>
-    <row r="72" spans="1:27">
+    <row r="72" spans="1:27" hidden="1" x14ac:dyDescent="0.5">
       <c r="A72" t="s">
         <v>2</v>
       </c>
@@ -4368,7 +4429,7 @@
         <v>0.22500000000000001</v>
       </c>
     </row>
-    <row r="73" spans="1:27">
+    <row r="73" spans="1:27" hidden="1" x14ac:dyDescent="0.5">
       <c r="A73" t="s">
         <v>2</v>
       </c>
@@ -4419,7 +4480,7 @@
         <v>0.315</v>
       </c>
     </row>
-    <row r="74" spans="1:27">
+    <row r="74" spans="1:27" hidden="1" x14ac:dyDescent="0.5">
       <c r="A74" t="s">
         <v>2</v>
       </c>
@@ -4470,7 +4531,7 @@
         <v>0.26800000000000002</v>
       </c>
     </row>
-    <row r="75" spans="1:27">
+    <row r="75" spans="1:27" hidden="1" x14ac:dyDescent="0.5">
       <c r="A75" t="s">
         <v>2</v>
       </c>
@@ -4521,7 +4582,7 @@
         <v>4.3200000000000002E-2</v>
       </c>
     </row>
-    <row r="76" spans="1:27">
+    <row r="76" spans="1:27" hidden="1" x14ac:dyDescent="0.5">
       <c r="A76" t="s">
         <v>2</v>
       </c>
@@ -4572,7 +4633,7 @@
         <v>330</v>
       </c>
     </row>
-    <row r="77" spans="1:27">
+    <row r="77" spans="1:27" hidden="1" x14ac:dyDescent="0.5">
       <c r="A77" t="s">
         <v>2</v>
       </c>
@@ -4641,7 +4702,7 @@
         <v>0.19397557124088433</v>
       </c>
     </row>
-    <row r="78" spans="1:27">
+    <row r="78" spans="1:27" hidden="1" x14ac:dyDescent="0.5">
       <c r="A78" t="s">
         <v>2</v>
       </c>
@@ -4707,7 +4768,7 @@
         <v>0.78</v>
       </c>
     </row>
-    <row r="79" spans="1:27">
+    <row r="79" spans="1:27" hidden="1" x14ac:dyDescent="0.5">
       <c r="A79" t="s">
         <v>2</v>
       </c>
@@ -4764,7 +4825,7 @@
         <v>0.3</v>
       </c>
     </row>
-    <row r="80" spans="1:27">
+    <row r="80" spans="1:27" hidden="1" x14ac:dyDescent="0.5">
       <c r="A80" t="s">
         <v>2</v>
       </c>
@@ -4819,7 +4880,7 @@
         <v>3.6000000000000004E-2</v>
       </c>
     </row>
-    <row r="81" spans="1:27">
+    <row r="81" spans="1:27" hidden="1" x14ac:dyDescent="0.5">
       <c r="A81" t="s">
         <v>2</v>
       </c>
@@ -4867,7 +4928,7 @@
         <v>9.0000000000000011E-3</v>
       </c>
     </row>
-    <row r="82" spans="1:27">
+    <row r="82" spans="1:27" hidden="1" x14ac:dyDescent="0.5">
       <c r="A82" t="s">
         <v>2</v>
       </c>
@@ -4907,7 +4968,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="83" spans="1:27">
+    <row r="83" spans="1:27" hidden="1" x14ac:dyDescent="0.5">
       <c r="A83" t="s">
         <v>2</v>
       </c>
@@ -4974,7 +5035,7 @@
         <v>0.13500000000000001</v>
       </c>
     </row>
-    <row r="84" spans="1:27">
+    <row r="84" spans="1:27" hidden="1" x14ac:dyDescent="0.5">
       <c r="A84" t="s">
         <v>2</v>
       </c>
@@ -5041,7 +5102,7 @@
         <v>0.08</v>
       </c>
     </row>
-    <row r="85" spans="1:27">
+    <row r="85" spans="1:27" hidden="1" x14ac:dyDescent="0.5">
       <c r="A85" t="s">
         <v>2</v>
       </c>
@@ -5078,7 +5139,7 @@
         <v>3.0281690140845072E-2</v>
       </c>
     </row>
-    <row r="86" spans="1:27">
+    <row r="86" spans="1:27" hidden="1" x14ac:dyDescent="0.5">
       <c r="A86" t="s">
         <v>2</v>
       </c>
@@ -5116,7 +5177,7 @@
       </c>
       <c r="Y86" s="15"/>
     </row>
-    <row r="87" spans="1:27">
+    <row r="87" spans="1:27" hidden="1" x14ac:dyDescent="0.5">
       <c r="A87" t="s">
         <v>2</v>
       </c>
@@ -5179,7 +5240,7 @@
         <v>2.1600000000000001E-2</v>
       </c>
     </row>
-    <row r="88" spans="1:27">
+    <row r="88" spans="1:27" hidden="1" x14ac:dyDescent="0.5">
       <c r="A88" t="s">
         <v>2</v>
       </c>
@@ -5246,7 +5307,7 @@
         <v>0.04</v>
       </c>
     </row>
-    <row r="89" spans="1:27">
+    <row r="89" spans="1:27" hidden="1" x14ac:dyDescent="0.5">
       <c r="A89" t="s">
         <v>2</v>
       </c>
@@ -5313,7 +5374,7 @@
         <v>125</v>
       </c>
     </row>
-    <row r="90" spans="1:27">
+    <row r="90" spans="1:27" hidden="1" x14ac:dyDescent="0.5">
       <c r="A90" t="s">
         <v>2</v>
       </c>
@@ -5365,7 +5426,7 @@
         <v>10.1</v>
       </c>
     </row>
-    <row r="91" spans="1:27">
+    <row r="91" spans="1:27" hidden="1" x14ac:dyDescent="0.5">
       <c r="A91" t="s">
         <v>2</v>
       </c>
@@ -5421,7 +5482,7 @@
         <v>1.4285714285714288</v>
       </c>
     </row>
-    <row r="92" spans="1:27">
+    <row r="92" spans="1:27" hidden="1" x14ac:dyDescent="0.5">
       <c r="A92" t="s">
         <v>2</v>
       </c>
@@ -5454,7 +5515,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="93" spans="1:27">
+    <row r="93" spans="1:27" hidden="1" x14ac:dyDescent="0.5">
       <c r="A93" t="s">
         <v>2</v>
       </c>
@@ -5486,7 +5547,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="94" spans="1:27">
+    <row r="94" spans="1:27" hidden="1" x14ac:dyDescent="0.5">
       <c r="A94" t="s">
         <v>2</v>
       </c>
@@ -5518,7 +5579,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="95" spans="1:27">
+    <row r="95" spans="1:27" hidden="1" x14ac:dyDescent="0.5">
       <c r="A95" t="s">
         <v>2</v>
       </c>
@@ -5550,7 +5611,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="96" spans="1:27">
+    <row r="96" spans="1:27" hidden="1" x14ac:dyDescent="0.5">
       <c r="A96" t="s">
         <v>2</v>
       </c>
@@ -5582,7 +5643,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="97" spans="1:26">
+    <row r="97" spans="1:26" hidden="1" x14ac:dyDescent="0.5">
       <c r="A97" t="s">
         <v>2</v>
       </c>
@@ -5614,7 +5675,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="98" spans="1:26">
+    <row r="98" spans="1:26" hidden="1" x14ac:dyDescent="0.5">
       <c r="A98" t="s">
         <v>2</v>
       </c>
@@ -5646,7 +5707,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="99" spans="1:26">
+    <row r="99" spans="1:26" hidden="1" x14ac:dyDescent="0.5">
       <c r="A99" t="s">
         <v>2</v>
       </c>
@@ -5680,7 +5741,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="100" spans="1:26">
+    <row r="100" spans="1:26" hidden="1" x14ac:dyDescent="0.5">
       <c r="A100" t="s">
         <v>2</v>
       </c>
@@ -5737,7 +5798,7 @@
         <v>0.34033613445378152</v>
       </c>
     </row>
-    <row r="101" spans="1:26">
+    <row r="101" spans="1:26" hidden="1" x14ac:dyDescent="0.5">
       <c r="A101" t="s">
         <v>2</v>
       </c>
@@ -5750,9 +5811,8 @@
       <c r="D101" t="s">
         <v>77</v>
       </c>
-      <c r="E101" t="str">
-        <f t="shared" si="0"/>
-        <v>Steam</v>
+      <c r="E101" t="s">
+        <v>175</v>
       </c>
       <c r="F101" t="s">
         <v>136</v>
@@ -5765,7 +5825,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="102" spans="1:26">
+    <row r="102" spans="1:26" hidden="1" x14ac:dyDescent="0.5">
       <c r="A102" t="s">
         <v>2</v>
       </c>
@@ -5803,7 +5863,7 @@
         <v>7.56</v>
       </c>
     </row>
-    <row r="103" spans="1:26">
+    <row r="103" spans="1:26" hidden="1" x14ac:dyDescent="0.5">
       <c r="A103" t="s">
         <v>2</v>
       </c>
@@ -5837,7 +5897,7 @@
         <v>1.55925</v>
       </c>
     </row>
-    <row r="104" spans="1:26">
+    <row r="104" spans="1:26" hidden="1" x14ac:dyDescent="0.5">
       <c r="A104" t="s">
         <v>2</v>
       </c>
@@ -5866,7 +5926,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="105" spans="1:26">
+    <row r="105" spans="1:26" hidden="1" x14ac:dyDescent="0.5">
       <c r="A105" t="s">
         <v>2</v>
       </c>
@@ -5895,7 +5955,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="106" spans="1:26">
+    <row r="106" spans="1:26" hidden="1" x14ac:dyDescent="0.5">
       <c r="A106" t="s">
         <v>2</v>
       </c>
@@ -5924,7 +5984,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="107" spans="1:26">
+    <row r="107" spans="1:26" hidden="1" x14ac:dyDescent="0.5">
       <c r="A107" t="s">
         <v>2</v>
       </c>
@@ -5957,7 +6017,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="108" spans="1:26">
+    <row r="108" spans="1:26" hidden="1" x14ac:dyDescent="0.5">
       <c r="A108" t="s">
         <v>2</v>
       </c>
@@ -5986,7 +6046,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="109" spans="1:26">
+    <row r="109" spans="1:26" hidden="1" x14ac:dyDescent="0.5">
       <c r="A109" t="s">
         <v>2</v>
       </c>
@@ -6032,7 +6092,7 @@
         <v>0.3</v>
       </c>
     </row>
-    <row r="110" spans="1:26">
+    <row r="110" spans="1:26" hidden="1" x14ac:dyDescent="0.5">
       <c r="A110" t="s">
         <v>2</v>
       </c>
@@ -6074,7 +6134,7 @@
         <v>1.1363636363636365</v>
       </c>
     </row>
-    <row r="111" spans="1:26">
+    <row r="111" spans="1:26" hidden="1" x14ac:dyDescent="0.5">
       <c r="A111" t="s">
         <v>2</v>
       </c>
@@ -6112,7 +6172,7 @@
         <v>2.119718309859155E-2</v>
       </c>
     </row>
-    <row r="112" spans="1:26">
+    <row r="112" spans="1:26" hidden="1" x14ac:dyDescent="0.5">
       <c r="A112" t="s">
         <v>2</v>
       </c>
@@ -6145,7 +6205,7 @@
         <v>0.67899999999999994</v>
       </c>
     </row>
-    <row r="113" spans="1:27">
+    <row r="113" spans="1:27" hidden="1" x14ac:dyDescent="0.5">
       <c r="A113" t="s">
         <v>2</v>
       </c>
@@ -6181,7 +6241,7 @@
         <v>0.05</v>
       </c>
     </row>
-    <row r="114" spans="1:27">
+    <row r="114" spans="1:27" hidden="1" x14ac:dyDescent="0.5">
       <c r="A114" t="s">
         <v>2</v>
       </c>
@@ -6211,7 +6271,7 @@
         <v>3.0281690140845072E-2</v>
       </c>
     </row>
-    <row r="115" spans="1:27">
+    <row r="115" spans="1:27" hidden="1" x14ac:dyDescent="0.5">
       <c r="A115" t="s">
         <v>2</v>
       </c>
@@ -6243,7 +6303,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="116" spans="1:27">
+    <row r="116" spans="1:27" hidden="1" x14ac:dyDescent="0.5">
       <c r="A116" t="s">
         <v>2</v>
       </c>
@@ -6275,7 +6335,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="117" spans="1:27">
+    <row r="117" spans="1:27" hidden="1" x14ac:dyDescent="0.5">
       <c r="A117" t="s">
         <v>2</v>
       </c>
@@ -6328,7 +6388,7 @@
         <v>0.3</v>
       </c>
     </row>
-    <row r="118" spans="1:27">
+    <row r="118" spans="1:27" hidden="1" x14ac:dyDescent="0.5">
       <c r="A118" t="s">
         <v>2</v>
       </c>
@@ -6385,7 +6445,7 @@
         <v>1.2707999999999999</v>
       </c>
     </row>
-    <row r="119" spans="1:27">
+    <row r="119" spans="1:27" hidden="1" x14ac:dyDescent="0.5">
       <c r="A119" t="s">
         <v>2</v>
       </c>
@@ -6420,7 +6480,7 @@
       </c>
       <c r="Q119" s="17"/>
     </row>
-    <row r="120" spans="1:27">
+    <row r="120" spans="1:27" hidden="1" x14ac:dyDescent="0.5">
       <c r="A120" t="s">
         <v>2</v>
       </c>
@@ -6466,7 +6526,7 @@
         <v>1.4039999999999999</v>
       </c>
     </row>
-    <row r="121" spans="1:27">
+    <row r="121" spans="1:27" hidden="1" x14ac:dyDescent="0.5">
       <c r="A121" t="s">
         <v>2</v>
       </c>
@@ -6523,7 +6583,7 @@
         <v>1.1232</v>
       </c>
     </row>
-    <row r="122" spans="1:27">
+    <row r="122" spans="1:27" hidden="1" x14ac:dyDescent="0.5">
       <c r="A122" t="s">
         <v>2</v>
       </c>
@@ -6553,7 +6613,7 @@
         <v>0.35460000000000003</v>
       </c>
     </row>
-    <row r="123" spans="1:27">
+    <row r="123" spans="1:27" hidden="1" x14ac:dyDescent="0.5">
       <c r="A123" t="s">
         <v>2</v>
       </c>
@@ -6588,7 +6648,7 @@
         <v>0.35460000000000003</v>
       </c>
     </row>
-    <row r="124" spans="1:27">
+    <row r="124" spans="1:27" hidden="1" x14ac:dyDescent="0.5">
       <c r="A124" t="s">
         <v>2</v>
       </c>
@@ -6635,7 +6695,7 @@
         <v>180</v>
       </c>
     </row>
-    <row r="125" spans="1:27">
+    <row r="125" spans="1:27" hidden="1" x14ac:dyDescent="0.5">
       <c r="A125" t="s">
         <v>2</v>
       </c>
@@ -6688,7 +6748,7 @@
         <v>0.08</v>
       </c>
     </row>
-    <row r="126" spans="1:27">
+    <row r="126" spans="1:27" hidden="1" x14ac:dyDescent="0.5">
       <c r="A126" t="s">
         <v>2</v>
       </c>
@@ -6727,7 +6787,7 @@
         <v>25.7</v>
       </c>
     </row>
-    <row r="127" spans="1:27">
+    <row r="127" spans="1:27" hidden="1" x14ac:dyDescent="0.5">
       <c r="A127" t="s">
         <v>2</v>
       </c>
@@ -6783,7 +6843,7 @@
         <v>67</v>
       </c>
     </row>
-    <row r="128" spans="1:27">
+    <row r="128" spans="1:27" hidden="1" x14ac:dyDescent="0.5">
       <c r="A128" t="s">
         <v>2</v>
       </c>
@@ -6832,7 +6892,7 @@
         <v>0.8</v>
       </c>
     </row>
-    <row r="129" spans="1:27">
+    <row r="129" spans="1:27" hidden="1" x14ac:dyDescent="0.5">
       <c r="A129" t="s">
         <v>2</v>
       </c>
@@ -6881,7 +6941,7 @@
         <v>1.2</v>
       </c>
     </row>
-    <row r="130" spans="1:27">
+    <row r="130" spans="1:27" hidden="1" x14ac:dyDescent="0.5">
       <c r="A130" t="s">
         <v>2</v>
       </c>
@@ -6912,7 +6972,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="131" spans="1:27">
+    <row r="131" spans="1:27" hidden="1" x14ac:dyDescent="0.5">
       <c r="A131" t="s">
         <v>2</v>
       </c>
@@ -6961,7 +7021,7 @@
         <v>1.0000000000000001E-5</v>
       </c>
     </row>
-    <row r="132" spans="1:27">
+    <row r="132" spans="1:27" hidden="1" x14ac:dyDescent="0.5">
       <c r="A132" t="s">
         <v>2</v>
       </c>
@@ -6994,7 +7054,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="133" spans="1:27">
+    <row r="133" spans="1:27" hidden="1" x14ac:dyDescent="0.5">
       <c r="A133" t="s">
         <v>2</v>
       </c>
@@ -7028,7 +7088,7 @@
         <v>3.6</v>
       </c>
     </row>
-    <row r="134" spans="1:27">
+    <row r="134" spans="1:27" hidden="1" x14ac:dyDescent="0.5">
       <c r="A134" t="s">
         <v>2</v>
       </c>
@@ -7069,7 +7129,7 @@
         <v>0.36</v>
       </c>
     </row>
-    <row r="135" spans="1:27">
+    <row r="135" spans="1:27" hidden="1" x14ac:dyDescent="0.5">
       <c r="A135" t="s">
         <v>2</v>
       </c>
@@ -7108,7 +7168,7 @@
         <v>0.9</v>
       </c>
     </row>
-    <row r="136" spans="1:27">
+    <row r="136" spans="1:27" hidden="1" x14ac:dyDescent="0.5">
       <c r="A136" t="s">
         <v>29</v>
       </c>
@@ -7128,7 +7188,7 @@
         <v>0.47265002739006901</v>
       </c>
     </row>
-    <row r="137" spans="1:27">
+    <row r="137" spans="1:27" hidden="1" x14ac:dyDescent="0.5">
       <c r="A137" t="s">
         <v>2</v>
       </c>
@@ -7149,7 +7209,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="138" spans="1:27">
+    <row r="138" spans="1:27" hidden="1" x14ac:dyDescent="0.5">
       <c r="A138" t="s">
         <v>2</v>
       </c>
@@ -7176,7 +7236,7 @@
         <v>1.42</v>
       </c>
     </row>
-    <row r="139" spans="1:27">
+    <row r="139" spans="1:27" hidden="1" x14ac:dyDescent="0.5">
       <c r="A139" t="s">
         <v>2</v>
       </c>
@@ -7197,7 +7257,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="140" spans="1:27">
+    <row r="140" spans="1:27" hidden="1" x14ac:dyDescent="0.5">
       <c r="A140" t="s">
         <v>2</v>
       </c>
@@ -7221,7 +7281,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="141" spans="1:27">
+    <row r="141" spans="1:27" hidden="1" x14ac:dyDescent="0.5">
       <c r="A141" t="s">
         <v>2</v>
       </c>
@@ -7245,7 +7305,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="142" spans="1:27">
+    <row r="142" spans="1:27" hidden="1" x14ac:dyDescent="0.5">
       <c r="A142" t="s">
         <v>2</v>
       </c>
@@ -7272,7 +7332,7 @@
         <v>12.7</v>
       </c>
     </row>
-    <row r="143" spans="1:27">
+    <row r="143" spans="1:27" hidden="1" x14ac:dyDescent="0.5">
       <c r="A143" t="s">
         <v>2</v>
       </c>
@@ -7296,7 +7356,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="144" spans="1:27">
+    <row r="144" spans="1:27" hidden="1" x14ac:dyDescent="0.5">
       <c r="A144" t="s">
         <v>2</v>
       </c>
@@ -7320,7 +7380,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="145" spans="1:26">
+    <row r="145" spans="1:26" hidden="1" x14ac:dyDescent="0.5">
       <c r="A145" t="s">
         <v>2</v>
       </c>
@@ -7348,7 +7408,7 @@
         <v>0.89</v>
       </c>
     </row>
-    <row r="146" spans="1:26">
+    <row r="146" spans="1:26" hidden="1" x14ac:dyDescent="0.5">
       <c r="A146" t="s">
         <v>2</v>
       </c>
@@ -7372,7 +7432,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="147" spans="1:26">
+    <row r="147" spans="1:26" hidden="1" x14ac:dyDescent="0.5">
       <c r="A147" t="s">
         <v>2</v>
       </c>
@@ -7400,7 +7460,7 @@
         <v>0.83</v>
       </c>
     </row>
-    <row r="148" spans="1:26">
+    <row r="148" spans="1:26" hidden="1" x14ac:dyDescent="0.5">
       <c r="A148" t="s">
         <v>2</v>
       </c>
@@ -7427,7 +7487,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="149" spans="1:26">
+    <row r="149" spans="1:26" hidden="1" x14ac:dyDescent="0.5">
       <c r="A149" t="s">
         <v>2</v>
       </c>
@@ -7454,7 +7514,7 @@
         <v>1.51</v>
       </c>
     </row>
-    <row r="150" spans="1:26">
+    <row r="150" spans="1:26" hidden="1" x14ac:dyDescent="0.5">
       <c r="A150" t="s">
         <v>2</v>
       </c>
@@ -7479,7 +7539,7 @@
         <v>0.34033613445378152</v>
       </c>
     </row>
-    <row r="151" spans="1:26">
+    <row r="151" spans="1:26" hidden="1" x14ac:dyDescent="0.5">
       <c r="A151" t="s">
         <v>2</v>
       </c>
@@ -7506,7 +7566,7 @@
         <v>11.96</v>
       </c>
     </row>
-    <row r="152" spans="1:26">
+    <row r="152" spans="1:26" hidden="1" x14ac:dyDescent="0.5">
       <c r="A152" t="s">
         <v>2</v>
       </c>
@@ -7527,7 +7587,7 @@
         <v>1.906666666666667</v>
       </c>
     </row>
-    <row r="153" spans="1:26">
+    <row r="153" spans="1:26" hidden="1" x14ac:dyDescent="0.5">
       <c r="A153" t="s">
         <v>2</v>
       </c>
@@ -7549,7 +7609,7 @@
         <v>7.2</v>
       </c>
     </row>
-    <row r="154" spans="1:26">
+    <row r="154" spans="1:26" hidden="1" x14ac:dyDescent="0.5">
       <c r="A154" t="s">
         <v>2</v>
       </c>
@@ -7570,7 +7630,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="155" spans="1:26">
+    <row r="155" spans="1:26" hidden="1" x14ac:dyDescent="0.5">
       <c r="A155" t="s">
         <v>2</v>
       </c>
@@ -7595,7 +7655,7 @@
         <v>3.6</v>
       </c>
     </row>
-    <row r="156" spans="1:26">
+    <row r="156" spans="1:26" hidden="1" x14ac:dyDescent="0.5">
       <c r="A156" t="s">
         <v>2</v>
       </c>
@@ -7620,7 +7680,7 @@
         <v>0.36</v>
       </c>
     </row>
-    <row r="157" spans="1:26">
+    <row r="157" spans="1:26" hidden="1" x14ac:dyDescent="0.5">
       <c r="A157" t="s">
         <v>2</v>
       </c>
@@ -7642,7 +7702,7 @@
         <v>0.9</v>
       </c>
     </row>
-    <row r="158" spans="1:26">
+    <row r="158" spans="1:26" hidden="1" x14ac:dyDescent="0.5">
       <c r="A158" t="s">
         <v>2</v>
       </c>
@@ -7670,7 +7730,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="159" spans="1:26">
+    <row r="159" spans="1:26" hidden="1" x14ac:dyDescent="0.5">
       <c r="A159" t="s">
         <v>2</v>
       </c>
@@ -7699,7 +7759,7 @@
         <v>1.3350380259623991</v>
       </c>
     </row>
-    <row r="160" spans="1:26">
+    <row r="160" spans="1:26" hidden="1" x14ac:dyDescent="0.5">
       <c r="A160" t="s">
         <v>2</v>
       </c>
@@ -7727,7 +7787,7 @@
         <v>0.2</v>
       </c>
     </row>
-    <row r="161" spans="1:25">
+    <row r="161" spans="1:25" hidden="1" x14ac:dyDescent="0.5">
       <c r="A161" t="s">
         <v>2</v>
       </c>
@@ -7752,8 +7812,288 @@
         <v>1.0340519801751746</v>
       </c>
     </row>
+    <row r="281" spans="5:5" x14ac:dyDescent="0.5">
+      <c r="E281" t="s">
+        <v>177</v>
+      </c>
+    </row>
+    <row r="289" spans="6:8" x14ac:dyDescent="0.5">
+      <c r="F289">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="299" spans="6:8" x14ac:dyDescent="0.5">
+      <c r="G299">
+        <v>0</v>
+      </c>
+      <c r="H299" s="9" t="s">
+        <v>178</v>
+      </c>
+    </row>
+    <row r="678" spans="8:8" x14ac:dyDescent="0.5">
+      <c r="H678" s="9" t="s">
+        <v>179</v>
+      </c>
+    </row>
+    <row r="837" spans="8:8" x14ac:dyDescent="0.5">
+      <c r="H837" s="9" t="s">
+        <v>177</v>
+      </c>
+    </row>
+    <row r="864" spans="8:8" x14ac:dyDescent="0.5">
+      <c r="H864" s="9" t="s">
+        <v>180</v>
+      </c>
+    </row>
+    <row r="955" spans="8:8" x14ac:dyDescent="0.5">
+      <c r="H955" s="9" t="s">
+        <v>177</v>
+      </c>
+    </row>
+    <row r="1200" spans="8:8" x14ac:dyDescent="0.5">
+      <c r="H1200" s="9" t="s">
+        <v>181</v>
+      </c>
+    </row>
+    <row r="1201" spans="8:8" x14ac:dyDescent="0.5">
+      <c r="H1201" s="9" t="s">
+        <v>177</v>
+      </c>
+    </row>
+    <row r="1202" spans="8:8" x14ac:dyDescent="0.5">
+      <c r="H1202" s="9" t="s">
+        <v>180</v>
+      </c>
+    </row>
+    <row r="1308" spans="8:8" x14ac:dyDescent="0.5">
+      <c r="H1308" s="9" t="s">
+        <v>177</v>
+      </c>
+    </row>
+    <row r="1494" spans="8:8" x14ac:dyDescent="0.5">
+      <c r="H1494" s="9" t="s">
+        <v>177</v>
+      </c>
+    </row>
+    <row r="1724" spans="8:8" x14ac:dyDescent="0.5">
+      <c r="H1724" s="9">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="1725" spans="8:8" x14ac:dyDescent="0.5">
+      <c r="H1725" s="9" t="s">
+        <v>177</v>
+      </c>
+    </row>
+    <row r="1726" spans="8:8" x14ac:dyDescent="0.5">
+      <c r="H1726" s="9" t="s">
+        <v>177</v>
+      </c>
+    </row>
+    <row r="1752" spans="8:8" x14ac:dyDescent="0.5">
+      <c r="H1752" s="9" t="s">
+        <v>182</v>
+      </c>
+    </row>
+    <row r="1753" spans="8:8" x14ac:dyDescent="0.5">
+      <c r="H1753" s="9" t="s">
+        <v>183</v>
+      </c>
+    </row>
+    <row r="1754" spans="8:8" x14ac:dyDescent="0.5">
+      <c r="H1754" s="9" t="s">
+        <v>184</v>
+      </c>
+    </row>
+    <row r="1764" spans="8:8" x14ac:dyDescent="0.5">
+      <c r="H1764" s="9" t="s">
+        <v>177</v>
+      </c>
+    </row>
+    <row r="1815" spans="8:8" x14ac:dyDescent="0.5">
+      <c r="H1815" s="9" t="s">
+        <v>177</v>
+      </c>
+    </row>
+    <row r="1816" spans="8:8" x14ac:dyDescent="0.5">
+      <c r="H1816" s="9" t="s">
+        <v>177</v>
+      </c>
+    </row>
+    <row r="1873" spans="8:8" x14ac:dyDescent="0.5">
+      <c r="H1873" s="9" t="s">
+        <v>180</v>
+      </c>
+    </row>
+    <row r="1874" spans="8:8" x14ac:dyDescent="0.5">
+      <c r="H1874" s="9" t="s">
+        <v>180</v>
+      </c>
+    </row>
+    <row r="1877" spans="8:8" x14ac:dyDescent="0.5">
+      <c r="H1877" s="9" t="s">
+        <v>177</v>
+      </c>
+    </row>
+    <row r="1879" spans="8:8" x14ac:dyDescent="0.5">
+      <c r="H1879" s="9" t="s">
+        <v>180</v>
+      </c>
+    </row>
+    <row r="1880" spans="8:8" x14ac:dyDescent="0.5">
+      <c r="H1880" s="9" t="s">
+        <v>185</v>
+      </c>
+    </row>
+    <row r="1881" spans="8:8" x14ac:dyDescent="0.5">
+      <c r="H1881" s="9" t="s">
+        <v>186</v>
+      </c>
+    </row>
+    <row r="1882" spans="8:8" x14ac:dyDescent="0.5">
+      <c r="H1882" s="9" t="s">
+        <v>180</v>
+      </c>
+    </row>
+    <row r="1884" spans="8:8" x14ac:dyDescent="0.5">
+      <c r="H1884" s="9" t="s">
+        <v>177</v>
+      </c>
+    </row>
+    <row r="1903" spans="8:8" x14ac:dyDescent="0.5">
+      <c r="H1903" s="9" t="s">
+        <v>186</v>
+      </c>
+    </row>
+    <row r="1905" spans="8:8" x14ac:dyDescent="0.5">
+      <c r="H1905" s="9" t="s">
+        <v>187</v>
+      </c>
+    </row>
+    <row r="1908" spans="8:8" x14ac:dyDescent="0.5">
+      <c r="H1908" s="9" t="s">
+        <v>188</v>
+      </c>
+    </row>
+    <row r="1909" spans="8:8" x14ac:dyDescent="0.5">
+      <c r="H1909" s="9" t="s">
+        <v>177</v>
+      </c>
+    </row>
+    <row r="1911" spans="8:8" x14ac:dyDescent="0.5">
+      <c r="H1911" s="9" t="s">
+        <v>189</v>
+      </c>
+    </row>
+    <row r="1921" spans="8:8" x14ac:dyDescent="0.5">
+      <c r="H1921" s="9" t="s">
+        <v>190</v>
+      </c>
+    </row>
+    <row r="1922" spans="8:8" x14ac:dyDescent="0.5">
+      <c r="H1922" s="9">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="1974" spans="8:8" x14ac:dyDescent="0.5">
+      <c r="H1974" s="9" t="s">
+        <v>177</v>
+      </c>
+    </row>
+    <row r="1988" spans="8:8" x14ac:dyDescent="0.5">
+      <c r="H1988" s="9">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="2365" spans="8:8" x14ac:dyDescent="0.5">
+      <c r="H2365" s="9" t="s">
+        <v>177</v>
+      </c>
+    </row>
+    <row r="2383" spans="8:8" x14ac:dyDescent="0.5">
+      <c r="H2383" s="9" t="s">
+        <v>191</v>
+      </c>
+    </row>
+    <row r="2384" spans="8:8" x14ac:dyDescent="0.5">
+      <c r="H2384" s="9" t="s">
+        <v>177</v>
+      </c>
+    </row>
+    <row r="2386" spans="8:8" x14ac:dyDescent="0.5">
+      <c r="H2386" s="9" t="s">
+        <v>185</v>
+      </c>
+    </row>
+    <row r="2398" spans="8:8" x14ac:dyDescent="0.5">
+      <c r="H2398" s="9" t="s">
+        <v>192</v>
+      </c>
+    </row>
+    <row r="2400" spans="8:8" x14ac:dyDescent="0.5">
+      <c r="H2400" s="9" t="s">
+        <v>177</v>
+      </c>
+    </row>
+    <row r="2434" spans="8:8" x14ac:dyDescent="0.5">
+      <c r="H2434" s="9" t="s">
+        <v>177</v>
+      </c>
+    </row>
+    <row r="2450" spans="8:9" x14ac:dyDescent="0.5">
+      <c r="H2450" s="9" t="s">
+        <v>193</v>
+      </c>
+    </row>
+    <row r="2451" spans="8:9" x14ac:dyDescent="0.5">
+      <c r="H2451" s="9" t="s">
+        <v>177</v>
+      </c>
+    </row>
+    <row r="2456" spans="8:9" x14ac:dyDescent="0.5">
+      <c r="I2456" s="9" t="s">
+        <v>194</v>
+      </c>
+    </row>
+    <row r="2462" spans="8:9" x14ac:dyDescent="0.5">
+      <c r="I2462" s="9" t="s">
+        <v>189</v>
+      </c>
+    </row>
+    <row r="2464" spans="8:9" x14ac:dyDescent="0.5">
+      <c r="I2464" s="9" t="s">
+        <v>176</v>
+      </c>
+    </row>
+    <row r="2473" spans="9:9" x14ac:dyDescent="0.5">
+      <c r="I2473" s="9" t="s">
+        <v>177</v>
+      </c>
+    </row>
+    <row r="2479" spans="9:9" x14ac:dyDescent="0.5">
+      <c r="I2479" s="9" t="s">
+        <v>177</v>
+      </c>
+    </row>
+    <row r="2598" spans="9:9" x14ac:dyDescent="0.5">
+      <c r="I2598" s="9" t="s">
+        <v>177</v>
+      </c>
+    </row>
   </sheetData>
-  <autoFilter ref="A2:AB161" xr:uid="{F5E4BE5B-48FB-4F9E-83ED-5B539B3F5C30}"/>
+  <autoFilter ref="A2:AB161" xr:uid="{F5E4BE5B-48FB-4F9E-83ED-5B539B3F5C30}">
+    <filterColumn colId="0">
+      <filters>
+        <filter val="Parameters"/>
+      </filters>
+    </filterColumn>
+    <filterColumn colId="3">
+      <filters>
+        <filter val="Share of electricity purchased in total demand"/>
+        <filter val="Share of energy delivered with natural gas"/>
+      </filters>
+    </filterColumn>
+  </autoFilter>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
   <legacyDrawing r:id="rId2"/>
@@ -7770,8 +8110,8 @@
 </file>
 
 <file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
-<ct:contentTypeSchema xmlns:ct="http://schemas.microsoft.com/office/2006/metadata/contentType" xmlns:ma="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes" ct:_="" ma:_="" ma:contentTypeName="Document" ma:contentTypeID="0x0101001B4ECEDC51D0484091AFD4177D66ED73" ma:contentTypeVersion="" ma:contentTypeDescription="Create a new document." ma:contentTypeScope="" ma:versionID="319a675c9647c7594acaff66597be50a">
-  <xsd:schema xmlns:xsd="http://www.w3.org/2001/XMLSchema" xmlns:xs="http://www.w3.org/2001/XMLSchema" xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:ns2="b44fa922-a688-4301-8945-67f7597c9c55" xmlns:ns3="f6f44a7d-d6f5-4042-8792-19cb5f90fb06" targetNamespace="http://schemas.microsoft.com/office/2006/metadata/properties" ma:root="true" ma:fieldsID="88dc2720d39439db86350823647c6b2d" ns2:_="" ns3:_="">
+<ct:contentTypeSchema xmlns:ct="http://schemas.microsoft.com/office/2006/metadata/contentType" xmlns:ma="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes" ct:_="" ma:_="" ma:contentTypeName="Document" ma:contentTypeID="0x0101001B4ECEDC51D0484091AFD4177D66ED73" ma:contentTypeVersion="" ma:contentTypeDescription="Create a new document." ma:contentTypeScope="" ma:versionID="0cc653c178d9ffcb24786b6a9d53371f">
+  <xsd:schema xmlns:xsd="http://www.w3.org/2001/XMLSchema" xmlns:xs="http://www.w3.org/2001/XMLSchema" xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:ns2="b44fa922-a688-4301-8945-67f7597c9c55" xmlns:ns3="f6f44a7d-d6f5-4042-8792-19cb5f90fb06" targetNamespace="http://schemas.microsoft.com/office/2006/metadata/properties" ma:root="true" ma:fieldsID="3af53c5407280ad7b07c166bc7f6511a" ns2:_="" ns3:_="">
     <xsd:import namespace="b44fa922-a688-4301-8945-67f7597c9c55"/>
     <xsd:import namespace="f6f44a7d-d6f5-4042-8792-19cb5f90fb06"/>
     <xsd:element name="properties">
@@ -7790,6 +8130,8 @@
                 <xsd:element ref="ns2:MediaServiceOCR" minOccurs="0"/>
                 <xsd:element ref="ns2:MediaServiceGenerationTime" minOccurs="0"/>
                 <xsd:element ref="ns2:MediaServiceEventHashCode" minOccurs="0"/>
+                <xsd:element ref="ns2:MediaServiceDateTaken" minOccurs="0"/>
+                <xsd:element ref="ns2:MediaLengthInSeconds" minOccurs="0"/>
               </xsd:all>
             </xsd:complexType>
           </xsd:element>
@@ -7842,6 +8184,16 @@
     <xsd:element name="MediaServiceEventHashCode" ma:index="17" nillable="true" ma:displayName="MediaServiceEventHashCode" ma:hidden="true" ma:internalName="MediaServiceEventHashCode" ma:readOnly="true">
       <xsd:simpleType>
         <xsd:restriction base="dms:Text"/>
+      </xsd:simpleType>
+    </xsd:element>
+    <xsd:element name="MediaServiceDateTaken" ma:index="18" nillable="true" ma:displayName="MediaServiceDateTaken" ma:hidden="true" ma:internalName="MediaServiceDateTaken" ma:readOnly="true">
+      <xsd:simpleType>
+        <xsd:restriction base="dms:Text"/>
+      </xsd:simpleType>
+    </xsd:element>
+    <xsd:element name="MediaLengthInSeconds" ma:index="19" nillable="true" ma:displayName="MediaLengthInSeconds" ma:hidden="true" ma:internalName="MediaLengthInSeconds" ma:readOnly="true">
+      <xsd:simpleType>
+        <xsd:restriction base="dms:Unknown"/>
       </xsd:simpleType>
     </xsd:element>
   </xsd:schema>
@@ -8002,22 +8354,7 @@
 </file>
 
 <file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{DB25B099-1FAC-465C-8173-479800A6E319}">
-  <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/contentType"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes"/>
-    <ds:schemaRef ds:uri="http://www.w3.org/2001/XMLSchema"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
-    <ds:schemaRef ds:uri="b44fa922-a688-4301-8945-67f7597c9c55"/>
-    <ds:schemaRef ds:uri="f6f44a7d-d6f5-4042-8792-19cb5f90fb06"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/documentManagement/types"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
-    <ds:schemaRef ds:uri="http://schemas.openxmlformats.org/package/2006/metadata/core-properties"/>
-    <ds:schemaRef ds:uri="http://purl.org/dc/elements/1.1/"/>
-    <ds:schemaRef ds:uri="http://purl.org/dc/terms/"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/internal/obd"/>
-  </ds:schemaRefs>
-</ds:datastoreItem>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{23495B5A-77F8-4066-B0A8-BF365967A169}"/>
 </file>
 
 <file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>

</xml_diff>